<commit_message>
nmv 31 05 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926874D6-1194-436D-93D6-B1B202175747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE79CADC-19D6-4D8D-A861-C1B9E1A06350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4740,7 +4740,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4762,12 +4762,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4799,7 +4793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4953,13 +4947,7 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4974,13 +4962,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5266,9 +5251,9 @@
   <dimension ref="A1:V2728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2053" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2004" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="J2069" sqref="J2069:U2069"/>
+      <selection pane="bottomLeft" activeCell="J2020" sqref="J2020:V2020"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -12937,7 +12922,7 @@
         <f t="shared" si="9"/>
         <v>180</v>
       </c>
-      <c r="N181" s="37" t="s">
+      <c r="N181" s="50" t="s">
         <v>247</v>
       </c>
       <c r="O181" s="5"/>
@@ -12982,7 +12967,7 @@
         <f t="shared" si="9"/>
         <v>181</v>
       </c>
-      <c r="N182" s="37" t="s">
+      <c r="N182" s="50" t="s">
         <v>248</v>
       </c>
       <c r="O182" s="5"/>
@@ -34572,32 +34557,32 @@
       <c r="I819" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="J819" s="7">
+      <c r="J819" s="54">
         <v>17</v>
       </c>
-      <c r="K819" s="39">
+      <c r="K819" s="55">
         <f t="shared" si="37"/>
         <v>818</v>
       </c>
-      <c r="L819" s="39">
+      <c r="L819" s="55">
         <v>1</v>
       </c>
-      <c r="M819" s="39">
+      <c r="M819" s="55">
         <f t="shared" si="39"/>
         <v>101</v>
       </c>
-      <c r="N819" s="37" t="s">
+      <c r="N819" s="56" t="s">
         <v>518</v>
       </c>
-      <c r="O819" s="6" t="s">
+      <c r="O819" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="P819" s="6"/>
-      <c r="Q819" s="6"/>
-      <c r="R819" s="6"/>
-      <c r="S819" s="6"/>
-      <c r="T819" s="6"/>
-      <c r="U819" s="6"/>
+      <c r="P819" s="57"/>
+      <c r="Q819" s="57"/>
+      <c r="R819" s="57"/>
+      <c r="S819" s="57"/>
+      <c r="T819" s="57"/>
+      <c r="U819" s="57"/>
       <c r="V819" s="37" t="s">
         <v>1226</v>
       </c>
@@ -41969,32 +41954,32 @@
       <c r="I1050" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="J1050" s="56">
+      <c r="J1050" s="7">
         <v>21</v>
       </c>
-      <c r="K1050" s="57">
+      <c r="K1050" s="39">
         <f t="shared" si="49"/>
         <v>1049</v>
       </c>
-      <c r="L1050" s="57">
+      <c r="L1050" s="39">
         <f t="shared" si="50"/>
         <v>50</v>
       </c>
-      <c r="M1050" s="57">
+      <c r="M1050" s="39">
         <f t="shared" si="51"/>
         <v>100</v>
       </c>
-      <c r="N1050" s="58" t="s">
+      <c r="N1050" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="O1050" s="59"/>
-      <c r="P1050" s="59"/>
-      <c r="Q1050" s="59"/>
-      <c r="R1050" s="59"/>
-      <c r="S1050" s="59"/>
-      <c r="T1050" s="59"/>
-      <c r="U1050" s="59"/>
-      <c r="V1050" s="58"/>
+      <c r="O1050" s="6"/>
+      <c r="P1050" s="6"/>
+      <c r="Q1050" s="6"/>
+      <c r="R1050" s="6"/>
+      <c r="S1050" s="6"/>
+      <c r="T1050" s="6"/>
+      <c r="U1050" s="6"/>
+      <c r="V1050" s="37"/>
     </row>
     <row r="1051" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1051" s="39" t="s">
@@ -47234,7 +47219,7 @@
         <f t="shared" si="57"/>
         <v>106</v>
       </c>
-      <c r="N1210" s="52" t="s">
+      <c r="N1210" s="56" t="s">
         <v>1522</v>
       </c>
       <c r="O1210" s="5"/>
@@ -48831,7 +48816,7 @@
         <f t="shared" si="60"/>
         <v>156</v>
       </c>
-      <c r="N1260" s="60" t="s">
+      <c r="N1260" s="53" t="s">
         <v>270</v>
       </c>
       <c r="O1260" s="6" t="s">
@@ -48866,7 +48851,7 @@
         <f t="shared" si="60"/>
         <v>157</v>
       </c>
-      <c r="N1261" s="60" t="s">
+      <c r="N1261" s="53" t="s">
         <v>668</v>
       </c>
       <c r="O1261" s="5"/>
@@ -70434,24 +70419,31 @@
       <c r="I2020" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="J2020" s="7">
+      <c r="J2020" s="43">
         <v>40</v>
       </c>
-      <c r="K2020" s="39">
+      <c r="K2020" s="42">
         <f t="shared" si="94"/>
         <v>2019</v>
       </c>
-      <c r="L2020" s="39">
+      <c r="L2020" s="42">
         <v>1</v>
       </c>
-      <c r="M2020" s="39">
+      <c r="M2020" s="42">
         <f t="shared" si="96"/>
         <v>51</v>
       </c>
-      <c r="N2020" s="37" t="s">
+      <c r="N2020" s="52" t="s">
         <v>339</v>
       </c>
-      <c r="V2020" s="37"/>
+      <c r="O2020" s="58"/>
+      <c r="P2020" s="59"/>
+      <c r="Q2020" s="59"/>
+      <c r="R2020" s="59"/>
+      <c r="S2020" s="59"/>
+      <c r="T2020" s="59"/>
+      <c r="U2020" s="59"/>
+      <c r="V2020" s="52"/>
     </row>
     <row r="2021" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I2021" s="39" t="s">
@@ -71635,31 +71627,24 @@
       <c r="I2069" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="J2069" s="53">
+      <c r="J2069" s="7">
         <v>40</v>
       </c>
-      <c r="K2069" s="54">
+      <c r="K2069" s="39">
         <f t="shared" si="97"/>
         <v>2068</v>
       </c>
-      <c r="L2069" s="54">
+      <c r="L2069" s="39">
         <f t="shared" si="98"/>
         <v>50</v>
       </c>
-      <c r="M2069" s="54">
+      <c r="M2069" s="39">
         <f t="shared" si="99"/>
         <v>100</v>
       </c>
-      <c r="N2069" s="55" t="s">
+      <c r="N2069" s="37" t="s">
         <v>954</v>
       </c>
-      <c r="O2069" s="61"/>
-      <c r="P2069" s="62"/>
-      <c r="Q2069" s="62"/>
-      <c r="R2069" s="62"/>
-      <c r="S2069" s="62"/>
-      <c r="T2069" s="62"/>
-      <c r="U2069" s="62"/>
       <c r="V2069" s="37"/>
     </row>
     <row r="2070" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73320,9 +73305,6 @@
       </c>
       <c r="P2134" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="S2134" s="1">
-        <v>35.32</v>
       </c>
       <c r="V2134" s="37" t="s">
         <v>1496</v>

</xml_diff>

<commit_message>
nmv 15 07 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94BF724-F18C-4431-8664-7A73952AB211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D920761D-8F80-42EF-BDD2-9FCC5B5657EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6487" uniqueCount="1523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1523">
   <si>
     <t>Passage</t>
   </si>
@@ -5242,9 +5242,9 @@
   <dimension ref="A1:V2728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A918" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U177" sqref="U177"/>
+      <selection pane="bottomLeft" activeCell="U920" sqref="U920"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -37774,9 +37774,7 @@
       <c r="R920" s="6"/>
       <c r="S920" s="6"/>
       <c r="T920" s="6"/>
-      <c r="U920" s="6" t="s">
-        <v>1500</v>
-      </c>
+      <c r="U920" s="6"/>
       <c r="V920" s="36"/>
     </row>
     <row r="921" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 16 07 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571C2600-A4A8-43BE-A30E-8A485FFE04B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4B5516-7590-407D-8D87-3E4053C66833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5242,9 +5242,9 @@
   <dimension ref="A1:V2728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1391" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2003" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="G1405" sqref="G1405"/>
+      <selection pane="bottomLeft" activeCell="N2011" sqref="N2011"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -70192,8 +70192,8 @@
         <f t="shared" si="96"/>
         <v>42</v>
       </c>
-      <c r="N2011" s="36" t="s">
-        <v>356</v>
+      <c r="N2011" s="37" t="s">
+        <v>922</v>
       </c>
       <c r="O2011" s="6" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
nmv 28 11 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C620E4D1-6695-4ACF-A25B-4179576D017D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DF23DE-FDB3-4397-BF4E-B4784955A49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3744,9 +3744,6 @@
     <t>dvAda#SakapAlaq itiq dvAda#Sa - kaqpAqlaqH</t>
   </si>
   <si>
-    <t>dvAda#SAkShaqretiq dvAda#SA - aqkShaqrAq</t>
-  </si>
-  <si>
     <t>tRuqtIqyaqsaqvaqnamiti# tRutIya - saqvaqnam</t>
   </si>
   <si>
@@ -4597,6 +4594,9 @@
   </si>
   <si>
     <t>aqBica#ritaqvai</t>
+  </si>
+  <si>
+    <t>dvAda#SAkShaqretiq dvAda#Sa - aqkShaqrAq</t>
   </si>
 </sst>
 </file>
@@ -5241,10 +5241,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A536" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A992" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V550" sqref="V550"/>
+      <selection pane="bottomLeft" activeCell="V1008" sqref="V1008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6104,7 +6104,7 @@
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="36" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -6539,7 +6539,7 @@
         <v>19</v>
       </c>
       <c r="N20" s="36" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="9" t="s">
@@ -6551,7 +6551,7 @@
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
       <c r="V20" s="36" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -6838,7 +6838,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="V27" s="36" t="s">
         <v>1147</v>
@@ -6873,7 +6873,7 @@
         <v>27</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="O28" s="5"/>
       <c r="P28" s="9" t="s">
@@ -6885,7 +6885,7 @@
       <c r="T28" s="9"/>
       <c r="U28" s="9"/>
       <c r="V28" s="36" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="29" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -7281,7 +7281,7 @@
         <v>37</v>
       </c>
       <c r="N38" s="36" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="O38" s="6"/>
       <c r="P38" s="9" t="s">
@@ -7293,7 +7293,7 @@
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
       <c r="V38" s="36" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -7570,7 +7570,7 @@
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
       <c r="U45" s="54" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V45" s="36"/>
     </row>
@@ -7647,7 +7647,7 @@
         <v>46</v>
       </c>
       <c r="N47" s="36" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="O47" s="6"/>
       <c r="P47" s="9" t="s">
@@ -7659,7 +7659,7 @@
       <c r="T47" s="9"/>
       <c r="U47" s="9"/>
       <c r="V47" s="36" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8086,7 +8086,7 @@
         <v>57</v>
       </c>
       <c r="N58" s="36" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="O58" s="6"/>
       <c r="P58" s="9" t="s">
@@ -8098,7 +8098,7 @@
       <c r="T58" s="9"/>
       <c r="U58" s="9"/>
       <c r="V58" s="36" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8536,7 +8536,7 @@
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
       <c r="V69" s="36" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8623,10 +8623,10 @@
         <v>82</v>
       </c>
       <c r="T71" s="48" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="U71" s="9" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V71" s="36"/>
     </row>
@@ -8672,7 +8672,7 @@
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
       <c r="U72" s="54" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="V72" s="36" t="s">
         <v>1150</v>
@@ -8985,7 +8985,7 @@
         <v>79</v>
       </c>
       <c r="N80" s="36" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="O80" s="5"/>
       <c r="P80" s="9" t="s">
@@ -8997,7 +8997,7 @@
       <c r="T80" s="9"/>
       <c r="U80" s="9"/>
       <c r="V80" s="36" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="81" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9229,7 +9229,7 @@
         <v>85</v>
       </c>
       <c r="N86" s="36" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="O86" s="6"/>
       <c r="P86" s="9" t="s">
@@ -9241,7 +9241,7 @@
       <c r="T86" s="9"/>
       <c r="U86" s="9"/>
       <c r="V86" s="36" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="87" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9595,7 +9595,7 @@
         <v>94</v>
       </c>
       <c r="N95" s="36" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="O95" s="5"/>
       <c r="P95" s="9" t="s">
@@ -9607,7 +9607,7 @@
       <c r="T95" s="6"/>
       <c r="U95" s="6"/>
       <c r="V95" s="36" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="96" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9819,7 +9819,7 @@
         <v>100</v>
       </c>
       <c r="N101" s="36" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="O101" s="6" t="s">
         <v>74</v>
@@ -9833,7 +9833,7 @@
       <c r="T101" s="6"/>
       <c r="U101" s="6"/>
       <c r="V101" s="36" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="102" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10133,7 +10133,7 @@
       <c r="S109" s="6"/>
       <c r="T109" s="6"/>
       <c r="U109" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="V109" s="36"/>
     </row>
@@ -10162,7 +10162,7 @@
         <v>109</v>
       </c>
       <c r="N110" s="36" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="O110" s="5"/>
       <c r="P110" s="9" t="s">
@@ -10174,7 +10174,7 @@
       <c r="T110" s="6"/>
       <c r="U110" s="6"/>
       <c r="V110" s="36" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="111" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10364,7 +10364,7 @@
         <v>114</v>
       </c>
       <c r="N115" s="36" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="O115" s="5"/>
       <c r="P115" s="9" t="s">
@@ -10376,7 +10376,7 @@
       <c r="T115" s="6"/>
       <c r="U115" s="6"/>
       <c r="V115" s="36" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="116" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10731,7 +10731,7 @@
         <v>123</v>
       </c>
       <c r="N124" s="36" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="O124" s="5"/>
       <c r="P124" s="9" t="s">
@@ -10743,7 +10743,7 @@
       <c r="T124" s="6"/>
       <c r="U124" s="6"/>
       <c r="V124" s="36" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="125" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10855,7 +10855,7 @@
       <c r="S127" s="6"/>
       <c r="T127" s="6"/>
       <c r="U127" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="V127" s="36"/>
     </row>
@@ -10959,7 +10959,7 @@
         <v>129</v>
       </c>
       <c r="N130" s="36" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="O130" s="6" t="s">
         <v>74</v>
@@ -10973,7 +10973,7 @@
       <c r="T130" s="6"/>
       <c r="U130" s="6"/>
       <c r="V130" s="36" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="131" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11220,7 +11220,7 @@
         <v>136</v>
       </c>
       <c r="N137" s="36" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="O137" s="5"/>
       <c r="P137" s="9" t="s">
@@ -11232,7 +11232,7 @@
       <c r="T137" s="6"/>
       <c r="U137" s="6"/>
       <c r="V137" s="36" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="138" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11636,7 +11636,7 @@
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
       <c r="V148" s="36" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="149" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11791,7 +11791,7 @@
       <c r="S152" s="6"/>
       <c r="T152" s="6"/>
       <c r="U152" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V152" s="36" t="s">
         <v>1157</v>
@@ -12026,7 +12026,7 @@
         <v>157</v>
       </c>
       <c r="N158" s="36" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="O158" s="6"/>
       <c r="P158" s="9" t="s">
@@ -12038,7 +12038,7 @@
       <c r="T158" s="6"/>
       <c r="U158" s="6"/>
       <c r="V158" s="36" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="159" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12536,7 +12536,7 @@
       <c r="T171" s="6"/>
       <c r="U171" s="6"/>
       <c r="V171" s="36" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="172" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12645,7 +12645,7 @@
       <c r="S174" s="6"/>
       <c r="T174" s="6"/>
       <c r="U174" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="V174" s="36"/>
     </row>
@@ -12840,7 +12840,7 @@
       <c r="T179" s="6"/>
       <c r="U179" s="6"/>
       <c r="V179" s="36" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="180" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12964,10 +12964,10 @@
       <c r="Q182" s="6"/>
       <c r="R182" s="6"/>
       <c r="S182" s="6" t="s">
+        <v>1501</v>
+      </c>
+      <c r="T182" s="6" t="s">
         <v>1502</v>
-      </c>
-      <c r="T182" s="6" t="s">
-        <v>1503</v>
       </c>
       <c r="U182" s="6"/>
       <c r="V182" s="36"/>
@@ -13156,7 +13156,7 @@
         <v>186</v>
       </c>
       <c r="N187" s="36" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="O187" s="5"/>
       <c r="P187" s="9" t="s">
@@ -13168,7 +13168,7 @@
       <c r="T187" s="6"/>
       <c r="U187" s="6"/>
       <c r="V187" s="36" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="188" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13268,7 +13268,7 @@
         <v>189</v>
       </c>
       <c r="N190" s="36" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="O190" s="5"/>
       <c r="P190" s="9" t="s">
@@ -13280,7 +13280,7 @@
       <c r="T190" s="6"/>
       <c r="U190" s="6"/>
       <c r="V190" s="36" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="191" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13576,7 +13576,7 @@
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
       <c r="V198" s="36" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="199" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13677,7 +13677,7 @@
         <v>200</v>
       </c>
       <c r="N201" s="36" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="O201" s="5"/>
       <c r="P201" s="9" t="s">
@@ -13689,7 +13689,7 @@
       <c r="T201" s="6"/>
       <c r="U201" s="6"/>
       <c r="V201" s="36" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="202" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13940,7 +13940,7 @@
         <v>207</v>
       </c>
       <c r="N208" s="36" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="O208" s="5"/>
       <c r="P208" s="9" t="s">
@@ -13952,7 +13952,7 @@
       <c r="T208" s="6"/>
       <c r="U208" s="6"/>
       <c r="V208" s="36" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="209" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14106,7 +14106,7 @@
       <c r="T212" s="6"/>
       <c r="U212" s="6"/>
       <c r="V212" s="36" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="213" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14215,7 +14215,7 @@
       <c r="S215" s="6"/>
       <c r="T215" s="6"/>
       <c r="U215" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V215" s="36"/>
     </row>
@@ -14520,7 +14520,7 @@
       <c r="T223" s="6"/>
       <c r="U223" s="6"/>
       <c r="V223" s="36" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="224" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24436,7 +24436,7 @@
         <v>291</v>
       </c>
       <c r="N514" s="36" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="O514" s="6" t="s">
         <v>74</v>
@@ -24652,7 +24652,7 @@
       <c r="T520" s="6"/>
       <c r="U520" s="6"/>
       <c r="V520" s="36" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="521" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25660,7 +25660,7 @@
         <v>30</v>
       </c>
       <c r="N550" s="37" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="O550" s="6" t="s">
         <v>74</v>
@@ -28345,7 +28345,7 @@
         <v>108</v>
       </c>
       <c r="N628" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O628" s="6" t="s">
         <v>74</v>
@@ -28908,7 +28908,7 @@
         <v>124</v>
       </c>
       <c r="N644" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O644" s="6" t="s">
         <v>74</v>
@@ -29458,7 +29458,7 @@
         <v>140</v>
       </c>
       <c r="N660" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O660" s="6" t="s">
         <v>74</v>
@@ -31286,7 +31286,7 @@
     </row>
     <row r="718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A718" s="6" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="I718" s="38" t="s">
         <v>33</v>
@@ -31319,7 +31319,7 @@
       <c r="T718" s="6"/>
       <c r="U718" s="6"/>
       <c r="V718" s="36" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32550,7 +32550,7 @@
     </row>
     <row r="757" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A757" s="6" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="I757" s="38" t="s">
         <v>34</v>
@@ -38682,7 +38682,7 @@
     </row>
     <row r="950" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A950" s="6" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="I950" s="38" t="s">
         <v>38</v>
@@ -38703,7 +38703,7 @@
         <v>232</v>
       </c>
       <c r="N950" s="36" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="O950" s="5"/>
       <c r="P950" s="9" t="s">
@@ -38715,7 +38715,7 @@
       <c r="T950" s="6"/>
       <c r="U950" s="6"/>
       <c r="V950" s="36" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="951" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38977,7 +38977,7 @@
         <v>83</v>
       </c>
       <c r="T958" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="U958" s="6"/>
       <c r="V958" s="36"/>
@@ -40509,8 +40509,8 @@
       <c r="S1005" s="6"/>
       <c r="T1005" s="6"/>
       <c r="U1005" s="6"/>
-      <c r="V1005" s="36" t="s">
-        <v>1238</v>
+      <c r="V1005" s="37" t="s">
+        <v>1522</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40646,7 +40646,7 @@
       <c r="T1009" s="6"/>
       <c r="U1009" s="6"/>
       <c r="V1009" s="36" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1010" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40682,7 +40682,7 @@
       <c r="T1010" s="6"/>
       <c r="U1010" s="6"/>
       <c r="V1010" s="36" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1011" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41325,7 +41325,7 @@
       <c r="T1030" s="6"/>
       <c r="U1030" s="6"/>
       <c r="V1030" s="36" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1031" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41775,7 +41775,7 @@
       <c r="T1044" s="6"/>
       <c r="U1044" s="6"/>
       <c r="V1044" s="36" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1045" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42795,7 +42795,7 @@
       </c>
       <c r="U1076" s="6"/>
       <c r="V1076" s="36" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1077" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42864,7 +42864,7 @@
       <c r="T1078" s="6"/>
       <c r="U1078" s="6"/>
       <c r="V1078" s="36" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1079" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42962,7 +42962,7 @@
       <c r="T1081" s="6"/>
       <c r="U1081" s="6"/>
       <c r="V1081" s="36" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1082" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42998,7 +42998,7 @@
       <c r="T1082" s="6"/>
       <c r="U1082" s="6"/>
       <c r="V1082" s="36" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1083" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43162,7 +43162,7 @@
       <c r="T1087" s="6"/>
       <c r="U1087" s="6"/>
       <c r="V1087" s="36" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1088" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43683,7 +43683,7 @@
     </row>
     <row r="1104" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1104" s="6" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="H1104" s="25"/>
       <c r="I1104" s="38" t="s">
@@ -43717,7 +43717,7 @@
       <c r="T1104" s="6"/>
       <c r="U1104" s="6"/>
       <c r="V1104" s="36" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1105" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43881,7 +43881,7 @@
       <c r="T1109" s="6"/>
       <c r="U1109" s="6"/>
       <c r="V1109" s="36" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1110" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44197,7 +44197,7 @@
       <c r="T1119" s="6"/>
       <c r="U1119" s="6"/>
       <c r="V1119" s="36" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1120" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44445,7 +44445,7 @@
       <c r="T1126" s="6"/>
       <c r="U1126" s="6"/>
       <c r="V1126" s="36" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1127" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44699,7 +44699,7 @@
       <c r="T1134" s="6"/>
       <c r="U1134" s="6"/>
       <c r="V1134" s="36" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1135" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44735,7 +44735,7 @@
       <c r="T1135" s="6"/>
       <c r="U1135" s="6"/>
       <c r="V1135" s="36" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1136" spans="7:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44867,7 +44867,7 @@
       <c r="T1139" s="6"/>
       <c r="U1139" s="6"/>
       <c r="V1139" s="36" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1140" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45153,7 +45153,7 @@
       <c r="T1148" s="6"/>
       <c r="U1148" s="6"/>
       <c r="V1148" s="36" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1149" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45514,7 +45514,7 @@
       <c r="T1158" s="6"/>
       <c r="U1158" s="6"/>
       <c r="V1158" s="36" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1159" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45949,7 +45949,7 @@
       <c r="T1171" s="6"/>
       <c r="U1171" s="6"/>
       <c r="V1171" s="36" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1172" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46177,7 +46177,7 @@
       <c r="T1178" s="6"/>
       <c r="U1178" s="6"/>
       <c r="V1178" s="36" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1179" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46249,7 +46249,7 @@
       <c r="T1180" s="6"/>
       <c r="U1180" s="6"/>
       <c r="V1180" s="36" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="1181" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46355,7 +46355,7 @@
       <c r="T1183" s="6"/>
       <c r="U1183" s="6"/>
       <c r="V1183" s="36" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1184" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46390,7 +46390,7 @@
       <c r="T1184" s="6"/>
       <c r="U1184" s="6"/>
       <c r="V1184" s="36" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="1185" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46582,7 +46582,7 @@
       <c r="T1190" s="6"/>
       <c r="U1190" s="6"/>
       <c r="V1190" s="36" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1191" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46605,7 +46605,7 @@
         <v>87</v>
       </c>
       <c r="N1191" s="36" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="O1191" s="6" t="s">
         <v>74</v>
@@ -46617,7 +46617,7 @@
       <c r="T1191" s="6"/>
       <c r="U1191" s="6"/>
       <c r="V1191" s="36" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1192" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47207,7 +47207,7 @@
         <v>106</v>
       </c>
       <c r="N1210" s="36" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="O1210" s="5"/>
       <c r="P1210" s="6"/>
@@ -47547,7 +47547,7 @@
       <c r="T1220" s="6"/>
       <c r="U1220" s="6"/>
       <c r="V1220" s="36" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="1221" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47646,10 +47646,10 @@
       <c r="S1223" s="6"/>
       <c r="T1223" s="6"/>
       <c r="U1223" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="V1223" s="36" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1224" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47841,7 +47841,7 @@
       <c r="T1229" s="6"/>
       <c r="U1229" s="6"/>
       <c r="V1229" s="36" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1230" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47972,7 +47972,7 @@
       <c r="T1233" s="6"/>
       <c r="U1233" s="6"/>
       <c r="V1233" s="36" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1234" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48657,7 +48657,7 @@
       <c r="T1255" s="6"/>
       <c r="U1255" s="6"/>
       <c r="V1255" s="36" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1256" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48818,7 +48818,7 @@
     </row>
     <row r="1261" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1261" s="50" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="I1261" s="38" t="s">
         <v>45</v>
@@ -49228,7 +49228,7 @@
       <c r="T1273" s="6"/>
       <c r="U1273" s="6"/>
       <c r="V1273" s="36" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1274" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50511,7 +50511,7 @@
     </row>
     <row r="1314" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1314" s="6" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="C1314" s="30"/>
       <c r="I1314" s="38" t="s">
@@ -50545,7 +50545,7 @@
       <c r="T1314" s="6"/>
       <c r="U1314" s="6"/>
       <c r="V1314" s="36" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50707,7 +50707,7 @@
       <c r="T1319" s="6"/>
       <c r="U1319" s="6"/>
       <c r="V1319" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1320" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50904,7 +50904,7 @@
       <c r="T1325" s="6"/>
       <c r="U1325" s="6"/>
       <c r="V1325" s="36" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1326" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50941,7 +50941,7 @@
       <c r="T1326" s="6"/>
       <c r="U1326" s="6"/>
       <c r="V1326" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1327" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50978,7 +50978,7 @@
       <c r="T1327" s="6"/>
       <c r="U1327" s="6"/>
       <c r="V1327" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1328" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51349,7 +51349,7 @@
       <c r="T1338" s="6"/>
       <c r="U1338" s="6"/>
       <c r="V1338" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1339" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51385,7 +51385,7 @@
       <c r="T1339" s="6"/>
       <c r="U1339" s="6"/>
       <c r="V1339" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1340" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51581,7 +51581,7 @@
       <c r="T1345" s="6"/>
       <c r="U1345" s="6"/>
       <c r="V1345" s="36" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1346" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51617,7 +51617,7 @@
       <c r="T1346" s="6"/>
       <c r="U1346" s="6"/>
       <c r="V1346" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1347" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51653,7 +51653,7 @@
       <c r="T1347" s="6"/>
       <c r="U1347" s="6"/>
       <c r="V1347" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1348" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51989,7 +51989,7 @@
       <c r="T1357" s="6"/>
       <c r="U1357" s="6"/>
       <c r="V1357" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1358" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52026,7 +52026,7 @@
       <c r="T1358" s="6"/>
       <c r="U1358" s="6"/>
       <c r="V1358" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1359" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52096,7 +52096,7 @@
       <c r="T1360" s="6"/>
       <c r="U1360" s="6"/>
       <c r="V1360" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1361" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52230,7 +52230,7 @@
       <c r="T1364" s="6"/>
       <c r="U1364" s="6"/>
       <c r="V1364" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1365" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52374,7 +52374,7 @@
       <c r="T1368" s="6"/>
       <c r="U1368" s="6"/>
       <c r="V1368" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1369" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52412,7 +52412,7 @@
       <c r="T1369" s="6"/>
       <c r="U1369" s="6"/>
       <c r="V1369" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1370" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52482,7 +52482,7 @@
       <c r="T1371" s="6"/>
       <c r="U1371" s="6"/>
       <c r="V1371" s="36" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1372" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52616,7 +52616,7 @@
       <c r="T1375" s="6"/>
       <c r="U1375" s="6"/>
       <c r="V1375" s="36" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1376" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52684,7 +52684,7 @@
       <c r="T1377" s="6"/>
       <c r="U1377" s="6"/>
       <c r="V1377" s="37" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1378" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52753,7 +52753,7 @@
       <c r="T1379" s="6"/>
       <c r="U1379" s="6"/>
       <c r="V1379" s="37" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52897,7 +52897,7 @@
       <c r="T1383" s="6"/>
       <c r="U1383" s="6"/>
       <c r="V1383" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1384" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52933,7 +52933,7 @@
       <c r="T1384" s="6"/>
       <c r="U1384" s="6"/>
       <c r="V1384" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1385" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53001,7 +53001,7 @@
       <c r="T1386" s="6"/>
       <c r="U1386" s="6"/>
       <c r="V1386" s="36" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1387" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53369,7 +53369,7 @@
       <c r="T1397" s="6"/>
       <c r="U1397" s="6"/>
       <c r="V1397" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1398" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53405,7 +53405,7 @@
       <c r="T1398" s="6"/>
       <c r="U1398" s="6"/>
       <c r="V1398" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1399" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53473,7 +53473,7 @@
       <c r="T1400" s="6"/>
       <c r="U1400" s="6"/>
       <c r="V1400" s="36" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1401" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53596,7 +53596,7 @@
         <v>90</v>
       </c>
       <c r="N1404" s="37" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="O1404" s="6" t="s">
         <v>74</v>
@@ -53608,7 +53608,7 @@
       <c r="T1404" s="6"/>
       <c r="U1404" s="6"/>
       <c r="V1404" s="36" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1405" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53645,7 +53645,7 @@
       <c r="T1405" s="6"/>
       <c r="U1405" s="6"/>
       <c r="V1405" s="36" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1406" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53759,7 +53759,7 @@
       <c r="T1408" s="6"/>
       <c r="U1408" s="6"/>
       <c r="V1408" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1409" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53795,7 +53795,7 @@
       <c r="T1409" s="6"/>
       <c r="U1409" s="6"/>
       <c r="V1409" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1410" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53990,7 +53990,7 @@
       <c r="T1415" s="6"/>
       <c r="U1415" s="6"/>
       <c r="V1415" s="36" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1416" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54026,7 +54026,7 @@
       <c r="T1416" s="6"/>
       <c r="U1416" s="6"/>
       <c r="V1416" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1417" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54062,7 +54062,7 @@
       <c r="T1417" s="6"/>
       <c r="U1417" s="6"/>
       <c r="V1417" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1418" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54398,7 +54398,7 @@
       <c r="T1427" s="6"/>
       <c r="U1427" s="6"/>
       <c r="V1427" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1428" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54434,7 +54434,7 @@
       <c r="T1428" s="6"/>
       <c r="U1428" s="6"/>
       <c r="V1428" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1429" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55638,7 +55638,7 @@
       <c r="T1465" s="6"/>
       <c r="U1465" s="6"/>
       <c r="V1465" s="36" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1466" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56205,7 +56205,7 @@
       <c r="T1482" s="6"/>
       <c r="U1482" s="6"/>
       <c r="V1482" s="36" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1483" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56273,7 +56273,7 @@
       <c r="S1484" s="6"/>
       <c r="T1484" s="6"/>
       <c r="V1484" s="36" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1485" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56409,7 +56409,7 @@
       <c r="T1488" s="6"/>
       <c r="U1488" s="6"/>
       <c r="V1488" s="36" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1489" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56529,7 +56529,7 @@
         <v>178</v>
       </c>
       <c r="N1492" s="36" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="O1492" s="5"/>
       <c r="P1492" s="9" t="s">
@@ -56541,7 +56541,7 @@
       <c r="T1492" s="6"/>
       <c r="U1492" s="6"/>
       <c r="V1492" s="36" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1493" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56575,7 +56575,7 @@
       <c r="T1493" s="6"/>
       <c r="U1493" s="6"/>
       <c r="V1493" s="36" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1494" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56900,7 +56900,7 @@
       <c r="T1503" s="6"/>
       <c r="U1503" s="6"/>
       <c r="V1503" s="36" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1504" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56936,7 +56936,7 @@
       <c r="T1504" s="6"/>
       <c r="U1504" s="6"/>
       <c r="V1504" s="36" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1505" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57169,7 +57169,7 @@
       <c r="T1511" s="6"/>
       <c r="U1511" s="6"/>
       <c r="V1511" s="36" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1512" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57415,7 +57415,7 @@
       <c r="T1518" s="6"/>
       <c r="U1518" s="6"/>
       <c r="V1518" s="36" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1519" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57880,7 +57880,7 @@
       <c r="T1532" s="6"/>
       <c r="U1532" s="6"/>
       <c r="V1532" s="36" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1533" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58008,7 +58008,7 @@
       <c r="T1536" s="6"/>
       <c r="U1536" s="6"/>
       <c r="V1536" s="36" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1537" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58043,7 +58043,7 @@
       <c r="T1537" s="6"/>
       <c r="U1537" s="6"/>
       <c r="V1537" s="36" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1538" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58109,7 +58109,7 @@
       <c r="T1539" s="6"/>
       <c r="U1539" s="6"/>
       <c r="V1539" s="36" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1540" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58175,7 +58175,7 @@
       <c r="T1541" s="6"/>
       <c r="U1541" s="6"/>
       <c r="V1541" s="36" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1542" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58271,7 +58271,7 @@
       <c r="T1544" s="6"/>
       <c r="U1544" s="6"/>
       <c r="V1544" s="36" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1545" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58463,7 +58463,7 @@
       <c r="T1550" s="6"/>
       <c r="U1550" s="6"/>
       <c r="V1550" s="36" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1551" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58529,7 +58529,7 @@
       <c r="T1552" s="6"/>
       <c r="U1552" s="6"/>
       <c r="V1552" s="36" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1553" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58657,7 +58657,7 @@
       <c r="T1556" s="6"/>
       <c r="U1556" s="6"/>
       <c r="V1556" s="36" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1557" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58880,7 +58880,7 @@
       <c r="T1563" s="6"/>
       <c r="U1563" s="6"/>
       <c r="V1563" s="36" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1564" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59071,7 +59071,7 @@
       <c r="T1569" s="6"/>
       <c r="U1569" s="6"/>
       <c r="V1569" s="36" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1570" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59356,7 +59356,7 @@
       <c r="T1578" s="6"/>
       <c r="U1578" s="6"/>
       <c r="V1578" s="36" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1579" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59464,7 +59464,7 @@
         <v>74</v>
       </c>
       <c r="V1582" s="36" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1583" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59646,7 +59646,7 @@
         <v>74</v>
       </c>
       <c r="V1589" s="36" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1590" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59746,7 +59746,7 @@
         <v>74</v>
       </c>
       <c r="V1593" s="36" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1594" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59970,7 +59970,7 @@
         <v>74</v>
       </c>
       <c r="V1602" s="36" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1603" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60167,7 +60167,7 @@
         <v>74</v>
       </c>
       <c r="V1610" s="36" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60196,7 +60196,7 @@
         <v>74</v>
       </c>
       <c r="V1611" s="36" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60369,7 +60369,7 @@
         <v>74</v>
       </c>
       <c r="V1618" s="36" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1619" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60398,7 +60398,7 @@
         <v>74</v>
       </c>
       <c r="V1619" s="36" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1620" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60595,7 +60595,7 @@
         <v>74</v>
       </c>
       <c r="V1627" s="36" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1628" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61427,7 +61427,7 @@
         <v>74</v>
       </c>
       <c r="V1661" s="36" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1662" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61611,7 +61611,7 @@
         <v>74</v>
       </c>
       <c r="V1668" s="36" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1669" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61724,7 +61724,7 @@
         <v>74</v>
       </c>
       <c r="V1672" s="36" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1673" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61807,7 +61807,7 @@
         <v>74</v>
       </c>
       <c r="V1675" s="36" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1676" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61865,7 +61865,7 @@
         <v>76</v>
       </c>
       <c r="V1677" s="36" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1678" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62280,7 +62280,7 @@
         <v>76</v>
       </c>
       <c r="V1694" s="36" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1695" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62309,7 +62309,7 @@
         <v>74</v>
       </c>
       <c r="V1695" s="36" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1696" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62338,7 +62338,7 @@
         <v>74</v>
       </c>
       <c r="V1696" s="36" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="1697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62442,7 +62442,7 @@
         <v>110</v>
       </c>
       <c r="T1700" s="1" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="V1700" s="36"/>
     </row>
@@ -62571,7 +62571,7 @@
         <v>74</v>
       </c>
       <c r="V1705" s="36" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1706" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62672,7 +62672,7 @@
         <v>74</v>
       </c>
       <c r="V1709" s="36" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1710" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62965,7 +62965,7 @@
         <v>74</v>
       </c>
       <c r="V1721" s="36" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1722" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63162,7 +63162,7 @@
         <v>74</v>
       </c>
       <c r="V1729" s="36" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1730" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63750,7 +63750,7 @@
         <v>74</v>
       </c>
       <c r="V1753" s="36" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1754" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63827,7 +63827,7 @@
         <v>74</v>
       </c>
       <c r="V1756" s="36" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1757" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63856,7 +63856,7 @@
         <v>74</v>
       </c>
       <c r="V1757" s="36" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1758" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63885,7 +63885,7 @@
         <v>74</v>
       </c>
       <c r="V1758" s="36" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="1759" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64130,7 +64130,7 @@
         <v>78</v>
       </c>
       <c r="V1768" s="36" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1769" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64399,7 +64399,7 @@
     </row>
     <row r="1780" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1780" s="6" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="I1780" s="38" t="s">
         <v>54</v>
@@ -64501,7 +64501,7 @@
         <v>74</v>
       </c>
       <c r="V1783" s="36" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="1784" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64602,7 +64602,7 @@
         <v>74</v>
       </c>
       <c r="V1787" s="36" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="1788" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64895,13 +64895,13 @@
         <v>307</v>
       </c>
       <c r="N1799" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P1799" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V1799" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1800" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65192,7 +65192,7 @@
         <v>74</v>
       </c>
       <c r="V1811" s="36" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1812" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65322,7 +65322,7 @@
         <v>74</v>
       </c>
       <c r="V1816" s="36" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1817" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65519,7 +65519,7 @@
         <v>74</v>
       </c>
       <c r="V1824" s="36" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="1825" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65913,7 +65913,7 @@
         <v>74</v>
       </c>
       <c r="V1840" s="36" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1841" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65993,7 +65993,7 @@
         <v>83</v>
       </c>
       <c r="T1843" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V1843" s="36"/>
     </row>
@@ -66047,7 +66047,7 @@
         <v>74</v>
       </c>
       <c r="V1845" s="36" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1846" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66124,7 +66124,7 @@
         <v>74</v>
       </c>
       <c r="V1848" s="36" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1849" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67303,7 +67303,7 @@
         <v>74</v>
       </c>
       <c r="V1896" s="36" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1897" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67356,7 +67356,7 @@
         <v>74</v>
       </c>
       <c r="V1898" s="36" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1899" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67408,7 +67408,7 @@
         <v>74</v>
       </c>
       <c r="V1900" s="36" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1901" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67437,7 +67437,7 @@
         <v>74</v>
       </c>
       <c r="V1901" s="36" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1902" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67514,7 +67514,7 @@
         <v>74</v>
       </c>
       <c r="V1904" s="36" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="1905" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67615,7 +67615,7 @@
         <v>74</v>
       </c>
       <c r="V1908" s="36" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="1909" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67767,7 +67767,7 @@
         <v>74</v>
       </c>
       <c r="V1914" s="36" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1915" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67796,7 +67796,7 @@
         <v>74</v>
       </c>
       <c r="V1915" s="36" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1916" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68164,7 +68164,7 @@
         <v>74</v>
       </c>
       <c r="V1930" s="36" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1931" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68193,7 +68193,7 @@
         <v>74</v>
       </c>
       <c r="V1931" s="36" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1932" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68369,7 +68369,7 @@
         <v>74</v>
       </c>
       <c r="V1938" s="36" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1939" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69148,7 +69148,7 @@
         <v>75</v>
       </c>
       <c r="V1969" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1970" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69252,7 +69252,7 @@
         <v>74</v>
       </c>
       <c r="V1973" s="36" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1974" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69382,7 +69382,7 @@
         <v>74</v>
       </c>
       <c r="V1978" s="36" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1979" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69579,7 +69579,7 @@
         <v>74</v>
       </c>
       <c r="V1986" s="36" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1987" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69776,7 +69776,7 @@
         <v>74</v>
       </c>
       <c r="V1994" s="36" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1995" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69978,7 +69978,7 @@
         <v>74</v>
       </c>
       <c r="V2002" s="36" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="2003" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70199,7 +70199,7 @@
         <v>74</v>
       </c>
       <c r="V2011" s="36" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="2012" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71123,7 +71123,7 @@
         <v>74</v>
       </c>
       <c r="V2049" s="36" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="2050" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71194,13 +71194,13 @@
         <v>83</v>
       </c>
       <c r="N2052" s="37" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="O2052" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2052" s="36" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="2053" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71325,7 +71325,7 @@
         <v>74</v>
       </c>
       <c r="V2057" s="36" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="2058" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71432,7 +71432,7 @@
         <v>74</v>
       </c>
       <c r="V2061" s="36" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="2062" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71652,7 +71652,7 @@
         <v>74</v>
       </c>
       <c r="V2070" s="36" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="2071" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71753,7 +71753,7 @@
         <v>76</v>
       </c>
       <c r="V2074" s="36" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="2075" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71782,7 +71782,7 @@
         <v>74</v>
       </c>
       <c r="V2075" s="36" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="2076" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71835,7 +71835,7 @@
         <v>74</v>
       </c>
       <c r="V2077" s="36" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="2078" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72128,7 +72128,7 @@
         <v>74</v>
       </c>
       <c r="V2089" s="36" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="2090" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72313,7 +72313,7 @@
         <v>74</v>
       </c>
       <c r="V2096" s="37" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="2097" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72539,7 +72539,7 @@
         <v>74</v>
       </c>
       <c r="V2105" s="36" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="2106" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72568,7 +72568,7 @@
         <v>74</v>
       </c>
       <c r="V2106" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="2107" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72621,7 +72621,7 @@
         <v>74</v>
       </c>
       <c r="V2108" s="36" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="2109" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72650,7 +72650,7 @@
         <v>74</v>
       </c>
       <c r="V2109" s="36" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="2110" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72703,7 +72703,7 @@
         <v>74</v>
       </c>
       <c r="V2111" s="36" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="2112" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73260,7 +73260,7 @@
     </row>
     <row r="2134" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2134" s="6" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="I2134" s="38" t="s">
         <v>60</v>
@@ -73287,7 +73287,7 @@
         <v>75</v>
       </c>
       <c r="V2134" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2135" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73338,7 +73338,7 @@
         <v>74</v>
       </c>
       <c r="V2136" s="36" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="2137" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73367,7 +73367,7 @@
         <v>74</v>
       </c>
       <c r="V2137" s="36" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2138" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73420,7 +73420,7 @@
         <v>74</v>
       </c>
       <c r="V2139" s="36" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="2140" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73473,7 +73473,7 @@
         <v>74</v>
       </c>
       <c r="V2141" s="36" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="2142" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73502,7 +73502,7 @@
         <v>74</v>
       </c>
       <c r="V2142" s="36" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="2143" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73603,7 +73603,7 @@
         <v>74</v>
       </c>
       <c r="V2146" s="36" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="2147" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73632,7 +73632,7 @@
         <v>74</v>
       </c>
       <c r="V2147" s="36" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2148" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73685,7 +73685,7 @@
         <v>74</v>
       </c>
       <c r="V2149" s="36" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="2150" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73906,7 +73906,7 @@
         <v>74</v>
       </c>
       <c r="V2158" s="36" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="2159" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73935,7 +73935,7 @@
         <v>74</v>
       </c>
       <c r="V2159" s="36" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="2160" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73958,13 +73958,13 @@
         <v>26</v>
       </c>
       <c r="N2160" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2160" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2160" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74015,7 +74015,7 @@
         <v>74</v>
       </c>
       <c r="V2162" s="36" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="2163" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74044,7 +74044,7 @@
         <v>74</v>
       </c>
       <c r="V2163" s="36" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="2164" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74145,7 +74145,7 @@
         <v>74</v>
       </c>
       <c r="V2167" s="36" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="2168" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74264,13 +74264,13 @@
         <v>12</v>
       </c>
       <c r="N2172" s="36" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="O2172" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2172" s="36" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="2173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74293,13 +74293,13 @@
         <v>13</v>
       </c>
       <c r="N2173" s="37" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="O2173" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2173" s="36" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="2174" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74352,7 +74352,7 @@
         <v>74</v>
       </c>
       <c r="V2175" s="36" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="2176" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74573,7 +74573,7 @@
         <v>74</v>
       </c>
       <c r="V2184" s="36" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="2185" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74602,7 +74602,7 @@
         <v>74</v>
       </c>
       <c r="V2185" s="36" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="2186" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74625,13 +74625,13 @@
         <v>26</v>
       </c>
       <c r="N2186" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2186" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2186" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2187" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74658,7 +74658,7 @@
         <v>74</v>
       </c>
       <c r="V2187" s="36" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="2188" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74687,7 +74687,7 @@
         <v>74</v>
       </c>
       <c r="V2188" s="36" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="2189" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74716,7 +74716,7 @@
         <v>74</v>
       </c>
       <c r="V2189" s="36" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="2190" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74769,7 +74769,7 @@
         <v>74</v>
       </c>
       <c r="V2191" s="36" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="2192" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74801,7 +74801,7 @@
         <v>74</v>
       </c>
       <c r="V2192" s="36" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2193" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74833,7 +74833,7 @@
         <v>74</v>
       </c>
       <c r="V2193" s="36" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="2194" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74865,7 +74865,7 @@
         <v>74</v>
       </c>
       <c r="V2194" s="36" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="2195" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74918,7 +74918,7 @@
         <v>74</v>
       </c>
       <c r="V2196" s="36" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="2197" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74947,7 +74947,7 @@
         <v>74</v>
       </c>
       <c r="V2197" s="36" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="2198" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74976,7 +74976,7 @@
         <v>74</v>
       </c>
       <c r="V2198" s="36" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="2199" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75005,7 +75005,7 @@
         <v>74</v>
       </c>
       <c r="V2199" s="36" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="2200" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75154,7 +75154,7 @@
         <v>74</v>
       </c>
       <c r="V2205" s="36" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="2206" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75255,7 +75255,7 @@
         <v>74</v>
       </c>
       <c r="V2209" s="36" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="2210" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75284,7 +75284,7 @@
         <v>74</v>
       </c>
       <c r="V2210" s="36" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="2211" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75307,13 +75307,13 @@
         <v>25</v>
       </c>
       <c r="N2211" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2211" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2211" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2212" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75340,7 +75340,7 @@
         <v>74</v>
       </c>
       <c r="V2212" s="36" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="2213" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75441,7 +75441,7 @@
         <v>74</v>
       </c>
       <c r="V2216" s="36" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="2217" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75473,7 +75473,7 @@
         <v>74</v>
       </c>
       <c r="V2217" s="36" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="2218" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75505,7 +75505,7 @@
         <v>74</v>
       </c>
       <c r="V2218" s="36" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="2219" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75537,7 +75537,7 @@
         <v>74</v>
       </c>
       <c r="V2219" s="36" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="2220" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75593,7 +75593,7 @@
         <v>74</v>
       </c>
       <c r="V2221" s="36" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="2222" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75622,7 +75622,7 @@
         <v>74</v>
       </c>
       <c r="V2222" s="36" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="2223" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75651,7 +75651,7 @@
         <v>74</v>
       </c>
       <c r="V2223" s="36" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="2224" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75680,7 +75680,7 @@
         <v>74</v>
       </c>
       <c r="V2224" s="36" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="2225" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75733,7 +75733,7 @@
         <v>74</v>
       </c>
       <c r="V2226" s="36" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="2227" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75834,7 +75834,7 @@
         <v>74</v>
       </c>
       <c r="V2230" s="36" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="2231" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75911,7 +75911,7 @@
         <v>74</v>
       </c>
       <c r="V2233" s="36" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="2234" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75940,7 +75940,7 @@
         <v>74</v>
       </c>
       <c r="V2234" s="36" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="2235" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75969,7 +75969,7 @@
         <v>74</v>
       </c>
       <c r="V2235" s="36" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="2236" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75992,13 +75992,13 @@
         <v>25</v>
       </c>
       <c r="N2236" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2236" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2236" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2237" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76313,7 +76313,7 @@
         <v>74</v>
       </c>
       <c r="V2249" s="36" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="2250" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76411,7 +76411,7 @@
         <v>1042</v>
       </c>
       <c r="U2253" s="1" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V2253" s="36"/>
     </row>
@@ -76513,7 +76513,7 @@
         <v>74</v>
       </c>
       <c r="V2257" s="36" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="2258" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76542,12 +76542,12 @@
         <v>74</v>
       </c>
       <c r="V2258" s="36" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="2259" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2259" s="6" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="I2259" s="38" t="s">
         <v>65</v>
@@ -76568,13 +76568,13 @@
         <v>23</v>
       </c>
       <c r="N2259" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2259" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2259" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2260" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76673,7 +76673,7 @@
         <v>74</v>
       </c>
       <c r="V2263" s="36" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="2264" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76750,7 +76750,7 @@
         <v>74</v>
       </c>
       <c r="V2266" s="36" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="2267" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76851,7 +76851,7 @@
         <v>74</v>
       </c>
       <c r="V2270" s="36" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="2271" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76880,7 +76880,7 @@
         <v>74</v>
       </c>
       <c r="V2271" s="36" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="2272" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76957,7 +76957,7 @@
         <v>74</v>
       </c>
       <c r="V2274" s="36" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="2275" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77034,7 +77034,7 @@
         <v>74</v>
       </c>
       <c r="V2277" s="36" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="2278" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77063,7 +77063,7 @@
         <v>74</v>
       </c>
       <c r="V2278" s="36" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="2279" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77086,13 +77086,13 @@
         <v>20</v>
       </c>
       <c r="N2279" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2279" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2279" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2280" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77185,13 +77185,13 @@
         <v>4</v>
       </c>
       <c r="N2283" s="36" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="O2283" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2283" s="36" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="2284" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77244,7 +77244,7 @@
         <v>74</v>
       </c>
       <c r="V2285" s="36" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="2286" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77297,7 +77297,7 @@
         <v>74</v>
       </c>
       <c r="V2287" s="36" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="2288" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77350,7 +77350,7 @@
         <v>74</v>
       </c>
       <c r="V2289" s="36" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="2290" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77403,7 +77403,7 @@
         <v>74</v>
       </c>
       <c r="V2291" s="36" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="2292" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77624,7 +77624,7 @@
         <v>74</v>
       </c>
       <c r="V2300" s="36" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="2301" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77647,13 +77647,13 @@
         <v>22</v>
       </c>
       <c r="N2301" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2301" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2301" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2302" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77728,7 +77728,7 @@
         <v>74</v>
       </c>
       <c r="V2304" s="36" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="2305" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77805,7 +77805,7 @@
         <v>74</v>
       </c>
       <c r="V2307" s="36" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="2308" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77882,7 +77882,7 @@
         <v>74</v>
       </c>
       <c r="V2310" s="36" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="2311" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78055,7 +78055,7 @@
         <v>74</v>
       </c>
       <c r="V2317" s="36" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="2318" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78084,7 +78084,7 @@
         <v>74</v>
       </c>
       <c r="V2318" s="36" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="2319" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78107,13 +78107,13 @@
         <v>18</v>
       </c>
       <c r="N2319" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2319" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2319" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2320" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78332,7 +78332,7 @@
         <v>74</v>
       </c>
       <c r="V2328" s="36" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="2329" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78403,7 +78403,7 @@
         <v>12</v>
       </c>
       <c r="N2331" s="37" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="V2331" s="36"/>
     </row>
@@ -78529,7 +78529,7 @@
         <v>74</v>
       </c>
       <c r="V2336" s="36" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="2337" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78576,13 +78576,13 @@
         <v>19</v>
       </c>
       <c r="N2338" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2338" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2338" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78657,7 +78657,7 @@
         <v>74</v>
       </c>
       <c r="V2341" s="36" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="2342" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78758,7 +78758,7 @@
         <v>74</v>
       </c>
       <c r="V2345" s="36" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="2346" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78811,7 +78811,7 @@
         <v>74</v>
       </c>
       <c r="V2347" s="36" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="2348" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78864,7 +78864,7 @@
         <v>74</v>
       </c>
       <c r="V2349" s="36" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="2350" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78941,7 +78941,7 @@
         <v>74</v>
       </c>
       <c r="V2352" s="36" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="2353" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79018,7 +79018,7 @@
         <v>74</v>
       </c>
       <c r="V2355" s="36" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="2356" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79047,7 +79047,7 @@
         <v>74</v>
       </c>
       <c r="V2356" s="36" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="2357" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79076,12 +79076,12 @@
         <v>74</v>
       </c>
       <c r="V2357" s="36" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="2358" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2358" s="6" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="I2358" s="38" t="s">
         <v>70</v>
@@ -79102,13 +79102,13 @@
         <v>20</v>
       </c>
       <c r="N2358" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="P2358" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2358" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2359" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79159,7 +79159,7 @@
         <v>74</v>
       </c>
       <c r="V2360" s="36" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="2361" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79188,7 +79188,7 @@
         <v>74</v>
       </c>
       <c r="V2361" s="36" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="2362" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79241,7 +79241,7 @@
         <v>74</v>
       </c>
       <c r="V2363" s="36" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="2364" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79270,7 +79270,7 @@
         <v>74</v>
       </c>
       <c r="V2364" s="36" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="2365" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79323,7 +79323,7 @@
         <v>74</v>
       </c>
       <c r="V2366" s="36" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="2367" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79352,7 +79352,7 @@
         <v>74</v>
       </c>
       <c r="V2367" s="36" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="2368" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79381,7 +79381,7 @@
         <v>74</v>
       </c>
       <c r="V2368" s="36" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="2369" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79410,10 +79410,10 @@
         <v>76</v>
       </c>
       <c r="U2369" s="1" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V2369" s="36" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="2370" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79442,7 +79442,7 @@
         <v>76</v>
       </c>
       <c r="V2370" s="36" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="2371" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79471,7 +79471,7 @@
         <v>76</v>
       </c>
       <c r="V2371" s="36" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2372" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79500,7 +79500,7 @@
         <v>76</v>
       </c>
       <c r="V2372" s="36" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="2373" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79529,7 +79529,7 @@
         <v>74</v>
       </c>
       <c r="V2373" s="36" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="2374" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79558,7 +79558,7 @@
         <v>76</v>
       </c>
       <c r="V2374" s="36" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="2375" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79587,7 +79587,7 @@
         <v>76</v>
       </c>
       <c r="V2375" s="36" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="2376" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79616,7 +79616,7 @@
         <v>76</v>
       </c>
       <c r="V2376" s="36" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2377" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79645,7 +79645,7 @@
         <v>76</v>
       </c>
       <c r="V2377" s="36" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="2378" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79674,7 +79674,7 @@
         <v>76</v>
       </c>
       <c r="V2378" s="36" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="2379" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79703,7 +79703,7 @@
         <v>76</v>
       </c>
       <c r="V2379" s="36" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="2380" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79732,7 +79732,7 @@
         <v>76</v>
       </c>
       <c r="V2380" s="36" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="2381" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79761,7 +79761,7 @@
         <v>76</v>
       </c>
       <c r="V2381" s="36" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2382" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79790,7 +79790,7 @@
         <v>76</v>
       </c>
       <c r="V2382" s="36" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="2383" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79843,7 +79843,7 @@
         <v>74</v>
       </c>
       <c r="V2384" s="36" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="2385" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79896,7 +79896,7 @@
         <v>76</v>
       </c>
       <c r="V2386" s="36" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="2387" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79925,7 +79925,7 @@
         <v>76</v>
       </c>
       <c r="V2387" s="36" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="2388" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79954,7 +79954,7 @@
         <v>76</v>
       </c>
       <c r="V2388" s="36" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="2389" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79980,7 +79980,7 @@
         <v>1117</v>
       </c>
       <c r="U2389" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="V2389" s="36"/>
     </row>
@@ -80052,7 +80052,7 @@
         <v>34</v>
       </c>
       <c r="N2392" s="36" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="O2392" s="6" t="s">
         <v>74</v>
@@ -80061,7 +80061,7 @@
         <v>75</v>
       </c>
       <c r="V2392" s="36" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="2393" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80490,7 +80490,7 @@
         <v>74</v>
       </c>
       <c r="V2409" s="36" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="2410" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80567,7 +80567,7 @@
         <v>74</v>
       </c>
       <c r="V2412" s="36" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="2413" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80638,13 +80638,13 @@
         <v>23</v>
       </c>
       <c r="N2415" s="37" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="O2415" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2415" s="36" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="2416" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80700,7 +80700,7 @@
         <v>75</v>
       </c>
       <c r="V2417" s="36" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="2418" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81015,7 +81015,7 @@
         <v>74</v>
       </c>
       <c r="V2430" s="36" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="2431" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81092,7 +81092,7 @@
         <v>74</v>
       </c>
       <c r="V2433" s="36" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="2434" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81169,7 +81169,7 @@
         <v>74</v>
       </c>
       <c r="V2436" s="36" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="2437" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81192,7 +81192,7 @@
         <v>20</v>
       </c>
       <c r="N2437" s="36" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="O2437" s="6" t="s">
         <v>74</v>
@@ -81201,7 +81201,7 @@
         <v>75</v>
       </c>
       <c r="V2437" s="36" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="2438" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 30 11 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DF23DE-FDB3-4397-BF4E-B4784955A49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2487A111-4D2D-457F-8589-71E9E70C30DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1524">
   <si>
     <t>Passage</t>
   </si>
@@ -4401,9 +4401,6 @@
     <t>janA#nAqmitiq janA#nAm</t>
   </si>
   <si>
-    <t>Bavaqntvitiq Bava#nti</t>
-  </si>
-  <si>
     <t>maq iti# me</t>
   </si>
   <si>
@@ -4597,6 +4594,12 @@
   </si>
   <si>
     <t>dvAda#SAkShaqretiq dvAda#Sa - aqkShaqrAq</t>
+  </si>
+  <si>
+    <t>BavaqntItiq Bava#nti</t>
+  </si>
+  <si>
+    <t>naq iti# naH</t>
   </si>
 </sst>
 </file>
@@ -5242,9 +5245,9 @@
   <dimension ref="A1:V2728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A992" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1008" sqref="V1008"/>
+      <selection pane="bottomLeft" activeCell="P212" sqref="P212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6838,7 +6841,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V27" s="36" t="s">
         <v>1147</v>
@@ -6873,7 +6876,7 @@
         <v>27</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="O28" s="5"/>
       <c r="P28" s="9" t="s">
@@ -7570,7 +7573,7 @@
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
       <c r="U45" s="54" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V45" s="36"/>
     </row>
@@ -7658,8 +7661,8 @@
       <c r="S47" s="9"/>
       <c r="T47" s="9"/>
       <c r="U47" s="9"/>
-      <c r="V47" s="36" t="s">
-        <v>1457</v>
+      <c r="V47" s="37" t="s">
+        <v>1522</v>
       </c>
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8536,7 +8539,7 @@
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
       <c r="V69" s="36" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8623,10 +8626,10 @@
         <v>82</v>
       </c>
       <c r="T71" s="48" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="U71" s="9" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V71" s="36"/>
     </row>
@@ -8672,7 +8675,7 @@
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
       <c r="U72" s="54" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="V72" s="36" t="s">
         <v>1150</v>
@@ -8997,7 +9000,7 @@
       <c r="T80" s="9"/>
       <c r="U80" s="9"/>
       <c r="V80" s="36" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="81" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9241,7 +9244,7 @@
       <c r="T86" s="9"/>
       <c r="U86" s="9"/>
       <c r="V86" s="36" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="87" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9607,7 +9610,7 @@
       <c r="T95" s="6"/>
       <c r="U95" s="6"/>
       <c r="V95" s="36" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="96" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9833,7 +9836,7 @@
       <c r="T101" s="6"/>
       <c r="U101" s="6"/>
       <c r="V101" s="36" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="102" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10133,7 +10136,7 @@
       <c r="S109" s="6"/>
       <c r="T109" s="6"/>
       <c r="U109" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V109" s="36"/>
     </row>
@@ -10174,7 +10177,7 @@
       <c r="T110" s="6"/>
       <c r="U110" s="6"/>
       <c r="V110" s="36" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="111" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10376,7 +10379,7 @@
       <c r="T115" s="6"/>
       <c r="U115" s="6"/>
       <c r="V115" s="36" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="116" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10743,7 +10746,7 @@
       <c r="T124" s="6"/>
       <c r="U124" s="6"/>
       <c r="V124" s="36" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="125" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10855,7 +10858,7 @@
       <c r="S127" s="6"/>
       <c r="T127" s="6"/>
       <c r="U127" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V127" s="36"/>
     </row>
@@ -10973,7 +10976,7 @@
       <c r="T130" s="6"/>
       <c r="U130" s="6"/>
       <c r="V130" s="36" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="131" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11232,7 +11235,7 @@
       <c r="T137" s="6"/>
       <c r="U137" s="6"/>
       <c r="V137" s="36" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="138" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11636,7 +11639,7 @@
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
       <c r="V148" s="36" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="149" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11791,7 +11794,7 @@
       <c r="S152" s="6"/>
       <c r="T152" s="6"/>
       <c r="U152" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V152" s="36" t="s">
         <v>1157</v>
@@ -12038,7 +12041,7 @@
       <c r="T158" s="6"/>
       <c r="U158" s="6"/>
       <c r="V158" s="36" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="159" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12536,7 +12539,7 @@
       <c r="T171" s="6"/>
       <c r="U171" s="6"/>
       <c r="V171" s="36" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="172" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12645,7 +12648,7 @@
       <c r="S174" s="6"/>
       <c r="T174" s="6"/>
       <c r="U174" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V174" s="36"/>
     </row>
@@ -12840,7 +12843,7 @@
       <c r="T179" s="6"/>
       <c r="U179" s="6"/>
       <c r="V179" s="36" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="180" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12964,10 +12967,10 @@
       <c r="Q182" s="6"/>
       <c r="R182" s="6"/>
       <c r="S182" s="6" t="s">
+        <v>1500</v>
+      </c>
+      <c r="T182" s="6" t="s">
         <v>1501</v>
-      </c>
-      <c r="T182" s="6" t="s">
-        <v>1502</v>
       </c>
       <c r="U182" s="6"/>
       <c r="V182" s="36"/>
@@ -13168,7 +13171,7 @@
       <c r="T187" s="6"/>
       <c r="U187" s="6"/>
       <c r="V187" s="36" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="188" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13280,7 +13283,7 @@
       <c r="T190" s="6"/>
       <c r="U190" s="6"/>
       <c r="V190" s="36" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="191" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13576,7 +13579,7 @@
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
       <c r="V198" s="36" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="199" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13689,7 +13692,7 @@
       <c r="T201" s="6"/>
       <c r="U201" s="6"/>
       <c r="V201" s="36" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="202" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13952,7 +13955,7 @@
       <c r="T208" s="6"/>
       <c r="U208" s="6"/>
       <c r="V208" s="36" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="209" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14105,8 +14108,8 @@
       <c r="S212" s="6"/>
       <c r="T212" s="6"/>
       <c r="U212" s="6"/>
-      <c r="V212" s="36" t="s">
-        <v>1474</v>
+      <c r="V212" s="37" t="s">
+        <v>1523</v>
       </c>
     </row>
     <row r="213" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14215,7 +14218,7 @@
       <c r="S215" s="6"/>
       <c r="T215" s="6"/>
       <c r="U215" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V215" s="36"/>
     </row>
@@ -14520,7 +14523,7 @@
       <c r="T223" s="6"/>
       <c r="U223" s="6"/>
       <c r="V223" s="36" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="224" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24436,7 +24439,7 @@
         <v>291</v>
       </c>
       <c r="N514" s="36" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="O514" s="6" t="s">
         <v>74</v>
@@ -24652,7 +24655,7 @@
       <c r="T520" s="6"/>
       <c r="U520" s="6"/>
       <c r="V520" s="36" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="521" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25660,7 +25663,7 @@
         <v>30</v>
       </c>
       <c r="N550" s="37" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="O550" s="6" t="s">
         <v>74</v>
@@ -28345,7 +28348,7 @@
         <v>108</v>
       </c>
       <c r="N628" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="O628" s="6" t="s">
         <v>74</v>
@@ -28908,7 +28911,7 @@
         <v>124</v>
       </c>
       <c r="N644" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="O644" s="6" t="s">
         <v>74</v>
@@ -29458,7 +29461,7 @@
         <v>140</v>
       </c>
       <c r="N660" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="O660" s="6" t="s">
         <v>74</v>
@@ -31286,7 +31289,7 @@
     </row>
     <row r="718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A718" s="6" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="I718" s="38" t="s">
         <v>33</v>
@@ -31319,7 +31322,7 @@
       <c r="T718" s="6"/>
       <c r="U718" s="6"/>
       <c r="V718" s="36" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32550,7 +32553,7 @@
     </row>
     <row r="757" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A757" s="6" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="I757" s="38" t="s">
         <v>34</v>
@@ -38682,7 +38685,7 @@
     </row>
     <row r="950" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A950" s="6" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="I950" s="38" t="s">
         <v>38</v>
@@ -38715,7 +38718,7 @@
       <c r="T950" s="6"/>
       <c r="U950" s="6"/>
       <c r="V950" s="36" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="951" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38977,7 +38980,7 @@
         <v>83</v>
       </c>
       <c r="T958" s="6" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="U958" s="6"/>
       <c r="V958" s="36"/>
@@ -40510,7 +40513,7 @@
       <c r="T1005" s="6"/>
       <c r="U1005" s="6"/>
       <c r="V1005" s="37" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43683,7 +43686,7 @@
     </row>
     <row r="1104" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1104" s="6" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="H1104" s="25"/>
       <c r="I1104" s="38" t="s">
@@ -43717,7 +43720,7 @@
       <c r="T1104" s="6"/>
       <c r="U1104" s="6"/>
       <c r="V1104" s="36" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1105" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47207,7 +47210,7 @@
         <v>106</v>
       </c>
       <c r="N1210" s="36" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="O1210" s="5"/>
       <c r="P1210" s="6"/>
@@ -47646,7 +47649,7 @@
       <c r="S1223" s="6"/>
       <c r="T1223" s="6"/>
       <c r="U1223" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V1223" s="36" t="s">
         <v>1260</v>
@@ -48818,7 +48821,7 @@
     </row>
     <row r="1261" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1261" s="50" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="I1261" s="38" t="s">
         <v>45</v>
@@ -50511,7 +50514,7 @@
     </row>
     <row r="1314" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1314" s="6" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="C1314" s="30"/>
       <c r="I1314" s="38" t="s">
@@ -50545,7 +50548,7 @@
       <c r="T1314" s="6"/>
       <c r="U1314" s="6"/>
       <c r="V1314" s="36" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52684,7 +52687,7 @@
       <c r="T1377" s="6"/>
       <c r="U1377" s="6"/>
       <c r="V1377" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="1378" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52753,7 +52756,7 @@
       <c r="T1379" s="6"/>
       <c r="U1379" s="6"/>
       <c r="V1379" s="37" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53596,7 +53599,7 @@
         <v>90</v>
       </c>
       <c r="N1404" s="37" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="O1404" s="6" t="s">
         <v>74</v>
@@ -56541,7 +56544,7 @@
       <c r="T1492" s="6"/>
       <c r="U1492" s="6"/>
       <c r="V1492" s="36" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1493" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62442,7 +62445,7 @@
         <v>110</v>
       </c>
       <c r="T1700" s="1" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="V1700" s="36"/>
     </row>
@@ -64399,7 +64402,7 @@
     </row>
     <row r="1780" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1780" s="6" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="I1780" s="38" t="s">
         <v>54</v>
@@ -64901,7 +64904,7 @@
         <v>75</v>
       </c>
       <c r="V1799" s="36" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1800" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65993,7 +65996,7 @@
         <v>83</v>
       </c>
       <c r="T1843" s="6" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V1843" s="36"/>
     </row>
@@ -69148,7 +69151,7 @@
         <v>75</v>
       </c>
       <c r="V1969" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1970" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71194,7 +71197,7 @@
         <v>83</v>
       </c>
       <c r="N2052" s="37" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="O2052" s="6" t="s">
         <v>74</v>
@@ -73260,7 +73263,7 @@
     </row>
     <row r="2134" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2134" s="6" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="I2134" s="38" t="s">
         <v>60</v>
@@ -73287,7 +73290,7 @@
         <v>75</v>
       </c>
       <c r="V2134" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2135" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73964,7 +73967,7 @@
         <v>75</v>
       </c>
       <c r="V2160" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74293,7 +74296,7 @@
         <v>13</v>
       </c>
       <c r="N2173" s="37" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="O2173" s="6" t="s">
         <v>74</v>
@@ -74631,7 +74634,7 @@
         <v>75</v>
       </c>
       <c r="V2186" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2187" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75313,7 +75316,7 @@
         <v>75</v>
       </c>
       <c r="V2211" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2212" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75998,7 +76001,7 @@
         <v>75</v>
       </c>
       <c r="V2236" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2237" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76411,7 +76414,7 @@
         <v>1042</v>
       </c>
       <c r="U2253" s="1" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V2253" s="36"/>
     </row>
@@ -76547,7 +76550,7 @@
     </row>
     <row r="2259" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2259" s="6" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="I2259" s="38" t="s">
         <v>65</v>
@@ -76574,7 +76577,7 @@
         <v>75</v>
       </c>
       <c r="V2259" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2260" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77092,7 +77095,7 @@
         <v>75</v>
       </c>
       <c r="V2279" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2280" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77185,7 +77188,7 @@
         <v>4</v>
       </c>
       <c r="N2283" s="36" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="O2283" s="6" t="s">
         <v>74</v>
@@ -77653,7 +77656,7 @@
         <v>75</v>
       </c>
       <c r="V2301" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2302" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78113,7 +78116,7 @@
         <v>75</v>
       </c>
       <c r="V2319" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2320" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78403,7 +78406,7 @@
         <v>12</v>
       </c>
       <c r="N2331" s="37" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="V2331" s="36"/>
     </row>
@@ -78582,7 +78585,7 @@
         <v>75</v>
       </c>
       <c r="V2338" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79081,7 +79084,7 @@
     </row>
     <row r="2358" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2358" s="6" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="I2358" s="38" t="s">
         <v>70</v>
@@ -79108,7 +79111,7 @@
         <v>75</v>
       </c>
       <c r="V2358" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2359" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79410,7 +79413,7 @@
         <v>76</v>
       </c>
       <c r="U2369" s="1" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V2369" s="36" t="s">
         <v>1413</v>
@@ -79980,7 +79983,7 @@
         <v>1117</v>
       </c>
       <c r="U2389" s="1" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="V2389" s="36"/>
     </row>
@@ -80061,7 +80064,7 @@
         <v>75</v>
       </c>
       <c r="V2392" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2393" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80638,7 +80641,7 @@
         <v>23</v>
       </c>
       <c r="N2415" s="37" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="O2415" s="6" t="s">
         <v>74</v>
@@ -80700,7 +80703,7 @@
         <v>75</v>
       </c>
       <c r="V2417" s="36" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="2418" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81201,7 +81204,7 @@
         <v>75</v>
       </c>
       <c r="V2437" s="36" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="2438" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NMV 16 03 2025
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2487A111-4D2D-457F-8589-71E9E70C30DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55F9995-4F77-4B1D-9F31-BDC44676F86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1523">
   <si>
     <t>Passage</t>
   </si>
@@ -3988,9 +3988,6 @@
   </si>
   <si>
     <t>treqdhAqviqhiqtA iti# tredhA - viqhiqtAH</t>
-  </si>
-  <si>
-    <t>prAqjAqpaqtyA iti# prAjA - paqtyAqH</t>
   </si>
   <si>
     <t>vaiqSvaqkaqrmaqNIriti# vaiSva - kaqrmaqNIH</t>
@@ -5245,9 +5242,9 @@
   <dimension ref="A1:V2728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1889" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="P212" sqref="P212"/>
+      <selection pane="bottomLeft" activeCell="V1899" sqref="V1899"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6107,7 +6104,7 @@
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="36" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -6542,7 +6539,7 @@
         <v>19</v>
       </c>
       <c r="N20" s="36" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="9" t="s">
@@ -6554,7 +6551,7 @@
       <c r="T20" s="9"/>
       <c r="U20" s="9"/>
       <c r="V20" s="36" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="21" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -6841,7 +6838,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V27" s="36" t="s">
         <v>1147</v>
@@ -6876,7 +6873,7 @@
         <v>27</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="O28" s="5"/>
       <c r="P28" s="9" t="s">
@@ -6888,7 +6885,7 @@
       <c r="T28" s="9"/>
       <c r="U28" s="9"/>
       <c r="V28" s="36" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="29" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -7284,7 +7281,7 @@
         <v>37</v>
       </c>
       <c r="N38" s="36" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="O38" s="6"/>
       <c r="P38" s="9" t="s">
@@ -7296,7 +7293,7 @@
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
       <c r="V38" s="36" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -7573,7 +7570,7 @@
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
       <c r="U45" s="54" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V45" s="36"/>
     </row>
@@ -7650,7 +7647,7 @@
         <v>46</v>
       </c>
       <c r="N47" s="36" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="O47" s="6"/>
       <c r="P47" s="9" t="s">
@@ -7662,7 +7659,7 @@
       <c r="T47" s="9"/>
       <c r="U47" s="9"/>
       <c r="V47" s="37" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8089,7 +8086,7 @@
         <v>57</v>
       </c>
       <c r="N58" s="36" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="O58" s="6"/>
       <c r="P58" s="9" t="s">
@@ -8101,7 +8098,7 @@
       <c r="T58" s="9"/>
       <c r="U58" s="9"/>
       <c r="V58" s="36" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8539,7 +8536,7 @@
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
       <c r="V69" s="36" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8626,10 +8623,10 @@
         <v>82</v>
       </c>
       <c r="T71" s="48" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="U71" s="9" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V71" s="36"/>
     </row>
@@ -8675,7 +8672,7 @@
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
       <c r="U72" s="54" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="V72" s="36" t="s">
         <v>1150</v>
@@ -8988,7 +8985,7 @@
         <v>79</v>
       </c>
       <c r="N80" s="36" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="O80" s="5"/>
       <c r="P80" s="9" t="s">
@@ -9000,7 +8997,7 @@
       <c r="T80" s="9"/>
       <c r="U80" s="9"/>
       <c r="V80" s="36" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="81" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9232,7 +9229,7 @@
         <v>85</v>
       </c>
       <c r="N86" s="36" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="O86" s="6"/>
       <c r="P86" s="9" t="s">
@@ -9244,7 +9241,7 @@
       <c r="T86" s="9"/>
       <c r="U86" s="9"/>
       <c r="V86" s="36" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="87" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9598,7 +9595,7 @@
         <v>94</v>
       </c>
       <c r="N95" s="36" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="O95" s="5"/>
       <c r="P95" s="9" t="s">
@@ -9610,7 +9607,7 @@
       <c r="T95" s="6"/>
       <c r="U95" s="6"/>
       <c r="V95" s="36" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="96" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9822,7 +9819,7 @@
         <v>100</v>
       </c>
       <c r="N101" s="36" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="O101" s="6" t="s">
         <v>74</v>
@@ -9836,7 +9833,7 @@
       <c r="T101" s="6"/>
       <c r="U101" s="6"/>
       <c r="V101" s="36" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="102" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10136,7 +10133,7 @@
       <c r="S109" s="6"/>
       <c r="T109" s="6"/>
       <c r="U109" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V109" s="36"/>
     </row>
@@ -10165,7 +10162,7 @@
         <v>109</v>
       </c>
       <c r="N110" s="36" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="O110" s="5"/>
       <c r="P110" s="9" t="s">
@@ -10177,7 +10174,7 @@
       <c r="T110" s="6"/>
       <c r="U110" s="6"/>
       <c r="V110" s="36" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="111" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10367,7 +10364,7 @@
         <v>114</v>
       </c>
       <c r="N115" s="36" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="O115" s="5"/>
       <c r="P115" s="9" t="s">
@@ -10379,7 +10376,7 @@
       <c r="T115" s="6"/>
       <c r="U115" s="6"/>
       <c r="V115" s="36" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="116" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10734,7 +10731,7 @@
         <v>123</v>
       </c>
       <c r="N124" s="36" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="O124" s="5"/>
       <c r="P124" s="9" t="s">
@@ -10746,7 +10743,7 @@
       <c r="T124" s="6"/>
       <c r="U124" s="6"/>
       <c r="V124" s="36" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="125" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10858,7 +10855,7 @@
       <c r="S127" s="6"/>
       <c r="T127" s="6"/>
       <c r="U127" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V127" s="36"/>
     </row>
@@ -10962,7 +10959,7 @@
         <v>129</v>
       </c>
       <c r="N130" s="36" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="O130" s="6" t="s">
         <v>74</v>
@@ -10976,7 +10973,7 @@
       <c r="T130" s="6"/>
       <c r="U130" s="6"/>
       <c r="V130" s="36" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="131" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11223,7 +11220,7 @@
         <v>136</v>
       </c>
       <c r="N137" s="36" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="O137" s="5"/>
       <c r="P137" s="9" t="s">
@@ -11235,7 +11232,7 @@
       <c r="T137" s="6"/>
       <c r="U137" s="6"/>
       <c r="V137" s="36" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="138" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11639,7 +11636,7 @@
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
       <c r="V148" s="36" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="149" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11794,7 +11791,7 @@
       <c r="S152" s="6"/>
       <c r="T152" s="6"/>
       <c r="U152" s="6" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V152" s="36" t="s">
         <v>1157</v>
@@ -12029,7 +12026,7 @@
         <v>157</v>
       </c>
       <c r="N158" s="36" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="O158" s="6"/>
       <c r="P158" s="9" t="s">
@@ -12041,7 +12038,7 @@
       <c r="T158" s="6"/>
       <c r="U158" s="6"/>
       <c r="V158" s="36" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="159" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12539,7 +12536,7 @@
       <c r="T171" s="6"/>
       <c r="U171" s="6"/>
       <c r="V171" s="36" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="172" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12648,7 +12645,7 @@
       <c r="S174" s="6"/>
       <c r="T174" s="6"/>
       <c r="U174" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V174" s="36"/>
     </row>
@@ -12843,7 +12840,7 @@
       <c r="T179" s="6"/>
       <c r="U179" s="6"/>
       <c r="V179" s="36" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="180" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12967,10 +12964,10 @@
       <c r="Q182" s="6"/>
       <c r="R182" s="6"/>
       <c r="S182" s="6" t="s">
+        <v>1499</v>
+      </c>
+      <c r="T182" s="6" t="s">
         <v>1500</v>
-      </c>
-      <c r="T182" s="6" t="s">
-        <v>1501</v>
       </c>
       <c r="U182" s="6"/>
       <c r="V182" s="36"/>
@@ -13159,7 +13156,7 @@
         <v>186</v>
       </c>
       <c r="N187" s="36" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="O187" s="5"/>
       <c r="P187" s="9" t="s">
@@ -13171,7 +13168,7 @@
       <c r="T187" s="6"/>
       <c r="U187" s="6"/>
       <c r="V187" s="36" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="188" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13271,7 +13268,7 @@
         <v>189</v>
       </c>
       <c r="N190" s="36" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="O190" s="5"/>
       <c r="P190" s="9" t="s">
@@ -13283,7 +13280,7 @@
       <c r="T190" s="6"/>
       <c r="U190" s="6"/>
       <c r="V190" s="36" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="191" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13579,7 +13576,7 @@
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
       <c r="V198" s="36" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="199" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13680,7 +13677,7 @@
         <v>200</v>
       </c>
       <c r="N201" s="36" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="O201" s="5"/>
       <c r="P201" s="9" t="s">
@@ -13692,7 +13689,7 @@
       <c r="T201" s="6"/>
       <c r="U201" s="6"/>
       <c r="V201" s="36" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="202" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13943,7 +13940,7 @@
         <v>207</v>
       </c>
       <c r="N208" s="36" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="O208" s="5"/>
       <c r="P208" s="9" t="s">
@@ -13955,7 +13952,7 @@
       <c r="T208" s="6"/>
       <c r="U208" s="6"/>
       <c r="V208" s="36" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="209" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14109,7 +14106,7 @@
       <c r="T212" s="6"/>
       <c r="U212" s="6"/>
       <c r="V212" s="37" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="213" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14218,7 +14215,7 @@
       <c r="S215" s="6"/>
       <c r="T215" s="6"/>
       <c r="U215" s="6" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V215" s="36"/>
     </row>
@@ -14523,7 +14520,7 @@
       <c r="T223" s="6"/>
       <c r="U223" s="6"/>
       <c r="V223" s="36" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="224" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24439,7 +24436,7 @@
         <v>291</v>
       </c>
       <c r="N514" s="36" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="O514" s="6" t="s">
         <v>74</v>
@@ -24655,7 +24652,7 @@
       <c r="T520" s="6"/>
       <c r="U520" s="6"/>
       <c r="V520" s="36" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="521" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25663,7 +25660,7 @@
         <v>30</v>
       </c>
       <c r="N550" s="37" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="O550" s="6" t="s">
         <v>74</v>
@@ -28348,7 +28345,7 @@
         <v>108</v>
       </c>
       <c r="N628" s="37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="O628" s="6" t="s">
         <v>74</v>
@@ -28911,7 +28908,7 @@
         <v>124</v>
       </c>
       <c r="N644" s="37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="O644" s="6" t="s">
         <v>74</v>
@@ -29461,7 +29458,7 @@
         <v>140</v>
       </c>
       <c r="N660" s="37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="O660" s="6" t="s">
         <v>74</v>
@@ -31289,7 +31286,7 @@
     </row>
     <row r="718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A718" s="6" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="I718" s="38" t="s">
         <v>33</v>
@@ -31322,7 +31319,7 @@
       <c r="T718" s="6"/>
       <c r="U718" s="6"/>
       <c r="V718" s="36" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32553,7 +32550,7 @@
     </row>
     <row r="757" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A757" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="I757" s="38" t="s">
         <v>34</v>
@@ -38685,7 +38682,7 @@
     </row>
     <row r="950" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A950" s="6" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="I950" s="38" t="s">
         <v>38</v>
@@ -38706,7 +38703,7 @@
         <v>232</v>
       </c>
       <c r="N950" s="36" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="O950" s="5"/>
       <c r="P950" s="9" t="s">
@@ -38718,7 +38715,7 @@
       <c r="T950" s="6"/>
       <c r="U950" s="6"/>
       <c r="V950" s="36" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="951" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38980,7 +38977,7 @@
         <v>83</v>
       </c>
       <c r="T958" s="6" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="U958" s="6"/>
       <c r="V958" s="36"/>
@@ -40513,7 +40510,7 @@
       <c r="T1005" s="6"/>
       <c r="U1005" s="6"/>
       <c r="V1005" s="37" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43686,7 +43683,7 @@
     </row>
     <row r="1104" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1104" s="6" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="H1104" s="25"/>
       <c r="I1104" s="38" t="s">
@@ -43720,7 +43717,7 @@
       <c r="T1104" s="6"/>
       <c r="U1104" s="6"/>
       <c r="V1104" s="36" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1105" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46608,7 +46605,7 @@
         <v>87</v>
       </c>
       <c r="N1191" s="36" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="O1191" s="6" t="s">
         <v>74</v>
@@ -47210,7 +47207,7 @@
         <v>106</v>
       </c>
       <c r="N1210" s="36" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="O1210" s="5"/>
       <c r="P1210" s="6"/>
@@ -47649,7 +47646,7 @@
       <c r="S1223" s="6"/>
       <c r="T1223" s="6"/>
       <c r="U1223" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V1223" s="36" t="s">
         <v>1260</v>
@@ -48821,7 +48818,7 @@
     </row>
     <row r="1261" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1261" s="50" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="I1261" s="38" t="s">
         <v>45</v>
@@ -50514,7 +50511,7 @@
     </row>
     <row r="1314" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1314" s="6" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="C1314" s="30"/>
       <c r="I1314" s="38" t="s">
@@ -50548,7 +50545,7 @@
       <c r="T1314" s="6"/>
       <c r="U1314" s="6"/>
       <c r="V1314" s="36" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52687,7 +52684,7 @@
       <c r="T1377" s="6"/>
       <c r="U1377" s="6"/>
       <c r="V1377" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1378" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52756,7 +52753,7 @@
       <c r="T1379" s="6"/>
       <c r="U1379" s="6"/>
       <c r="V1379" s="37" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53599,7 +53596,7 @@
         <v>90</v>
       </c>
       <c r="N1404" s="37" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="O1404" s="6" t="s">
         <v>74</v>
@@ -56532,7 +56529,7 @@
         <v>178</v>
       </c>
       <c r="N1492" s="36" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="O1492" s="5"/>
       <c r="P1492" s="9" t="s">
@@ -56544,7 +56541,7 @@
       <c r="T1492" s="6"/>
       <c r="U1492" s="6"/>
       <c r="V1492" s="36" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1493" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62445,7 +62442,7 @@
         <v>110</v>
       </c>
       <c r="T1700" s="1" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="V1700" s="36"/>
     </row>
@@ -64402,7 +64399,7 @@
     </row>
     <row r="1780" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1780" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="I1780" s="38" t="s">
         <v>54</v>
@@ -64898,13 +64895,13 @@
         <v>307</v>
       </c>
       <c r="N1799" s="36" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="P1799" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V1799" s="36" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1800" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65996,7 +65993,7 @@
         <v>83</v>
       </c>
       <c r="T1843" s="6" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="V1843" s="36"/>
     </row>
@@ -67358,8 +67355,8 @@
       <c r="O1898" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="V1898" s="36" t="s">
-        <v>1320</v>
+      <c r="V1898" s="37" t="s">
+        <v>1321</v>
       </c>
     </row>
     <row r="1899" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67411,7 +67408,7 @@
         <v>74</v>
       </c>
       <c r="V1900" s="36" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1901" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67517,7 +67514,7 @@
         <v>74</v>
       </c>
       <c r="V1904" s="36" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1905" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67618,7 +67615,7 @@
         <v>74</v>
       </c>
       <c r="V1908" s="36" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1909" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67770,7 +67767,7 @@
         <v>74</v>
       </c>
       <c r="V1914" s="36" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="1915" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67799,7 +67796,7 @@
         <v>74</v>
       </c>
       <c r="V1915" s="36" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1916" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68167,7 +68164,7 @@
         <v>74</v>
       </c>
       <c r="V1930" s="36" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1931" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68196,7 +68193,7 @@
         <v>74</v>
       </c>
       <c r="V1931" s="36" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1932" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68372,7 +68369,7 @@
         <v>74</v>
       </c>
       <c r="V1938" s="36" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1939" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69151,7 +69148,7 @@
         <v>75</v>
       </c>
       <c r="V1969" s="36" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1970" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69255,7 +69252,7 @@
         <v>74</v>
       </c>
       <c r="V1973" s="36" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1974" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69385,7 +69382,7 @@
         <v>74</v>
       </c>
       <c r="V1978" s="36" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1979" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69582,7 +69579,7 @@
         <v>74</v>
       </c>
       <c r="V1986" s="36" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1987" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69779,7 +69776,7 @@
         <v>74</v>
       </c>
       <c r="V1994" s="36" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1995" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69981,7 +69978,7 @@
         <v>74</v>
       </c>
       <c r="V2002" s="36" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="2003" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70202,7 +70199,7 @@
         <v>74</v>
       </c>
       <c r="V2011" s="36" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="2012" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71197,13 +71194,13 @@
         <v>83</v>
       </c>
       <c r="N2052" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O2052" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2052" s="36" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="2053" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71328,7 +71325,7 @@
         <v>74</v>
       </c>
       <c r="V2057" s="36" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="2058" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71435,7 +71432,7 @@
         <v>74</v>
       </c>
       <c r="V2061" s="36" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="2062" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71655,7 +71652,7 @@
         <v>74</v>
       </c>
       <c r="V2070" s="36" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="2071" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71785,7 +71782,7 @@
         <v>74</v>
       </c>
       <c r="V2075" s="36" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="2076" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71838,7 +71835,7 @@
         <v>74</v>
       </c>
       <c r="V2077" s="36" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="2078" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72131,7 +72128,7 @@
         <v>74</v>
       </c>
       <c r="V2089" s="36" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="2090" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72316,7 +72313,7 @@
         <v>74</v>
       </c>
       <c r="V2096" s="37" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="2097" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72653,7 +72650,7 @@
         <v>74</v>
       </c>
       <c r="V2109" s="36" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="2110" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72706,7 +72703,7 @@
         <v>74</v>
       </c>
       <c r="V2111" s="36" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="2112" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73263,7 +73260,7 @@
     </row>
     <row r="2134" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2134" s="6" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="I2134" s="38" t="s">
         <v>60</v>
@@ -73290,7 +73287,7 @@
         <v>75</v>
       </c>
       <c r="V2134" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2135" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73341,7 +73338,7 @@
         <v>74</v>
       </c>
       <c r="V2136" s="36" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="2137" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73370,7 +73367,7 @@
         <v>74</v>
       </c>
       <c r="V2137" s="36" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="2138" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73423,7 +73420,7 @@
         <v>74</v>
       </c>
       <c r="V2139" s="36" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="2140" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73476,7 +73473,7 @@
         <v>74</v>
       </c>
       <c r="V2141" s="36" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="2142" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73505,7 +73502,7 @@
         <v>74</v>
       </c>
       <c r="V2142" s="36" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="2143" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73606,7 +73603,7 @@
         <v>74</v>
       </c>
       <c r="V2146" s="36" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="2147" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73635,7 +73632,7 @@
         <v>74</v>
       </c>
       <c r="V2147" s="36" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="2148" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73688,7 +73685,7 @@
         <v>74</v>
       </c>
       <c r="V2149" s="36" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="2150" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73909,7 +73906,7 @@
         <v>74</v>
       </c>
       <c r="V2158" s="36" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="2159" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73938,7 +73935,7 @@
         <v>74</v>
       </c>
       <c r="V2159" s="36" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="2160" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73961,13 +73958,13 @@
         <v>26</v>
       </c>
       <c r="N2160" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2160" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2160" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74018,7 +74015,7 @@
         <v>74</v>
       </c>
       <c r="V2162" s="36" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="2163" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74047,7 +74044,7 @@
         <v>74</v>
       </c>
       <c r="V2163" s="36" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="2164" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74148,7 +74145,7 @@
         <v>74</v>
       </c>
       <c r="V2167" s="36" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="2168" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74267,13 +74264,13 @@
         <v>12</v>
       </c>
       <c r="N2172" s="36" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="O2172" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2172" s="36" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="2173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74296,13 +74293,13 @@
         <v>13</v>
       </c>
       <c r="N2173" s="37" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="O2173" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2173" s="36" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="2174" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74355,7 +74352,7 @@
         <v>74</v>
       </c>
       <c r="V2175" s="36" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="2176" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74576,7 +74573,7 @@
         <v>74</v>
       </c>
       <c r="V2184" s="36" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="2185" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74605,7 +74602,7 @@
         <v>74</v>
       </c>
       <c r="V2185" s="36" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="2186" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74628,13 +74625,13 @@
         <v>26</v>
       </c>
       <c r="N2186" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2186" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2186" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2187" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74661,7 +74658,7 @@
         <v>74</v>
       </c>
       <c r="V2187" s="36" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="2188" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74690,7 +74687,7 @@
         <v>74</v>
       </c>
       <c r="V2188" s="36" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="2189" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74719,7 +74716,7 @@
         <v>74</v>
       </c>
       <c r="V2189" s="36" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="2190" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74772,7 +74769,7 @@
         <v>74</v>
       </c>
       <c r="V2191" s="36" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="2192" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74804,7 +74801,7 @@
         <v>74</v>
       </c>
       <c r="V2192" s="36" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="2193" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74836,7 +74833,7 @@
         <v>74</v>
       </c>
       <c r="V2193" s="36" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2194" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74868,7 +74865,7 @@
         <v>74</v>
       </c>
       <c r="V2194" s="36" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="2195" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74921,7 +74918,7 @@
         <v>74</v>
       </c>
       <c r="V2196" s="36" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="2197" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74950,7 +74947,7 @@
         <v>74</v>
       </c>
       <c r="V2197" s="36" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="2198" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74979,7 +74976,7 @@
         <v>74</v>
       </c>
       <c r="V2198" s="36" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="2199" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75008,7 +75005,7 @@
         <v>74</v>
       </c>
       <c r="V2199" s="36" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="2200" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75157,7 +75154,7 @@
         <v>74</v>
       </c>
       <c r="V2205" s="36" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="2206" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75258,7 +75255,7 @@
         <v>74</v>
       </c>
       <c r="V2209" s="36" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="2210" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75287,7 +75284,7 @@
         <v>74</v>
       </c>
       <c r="V2210" s="36" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="2211" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75310,13 +75307,13 @@
         <v>25</v>
       </c>
       <c r="N2211" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2211" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2211" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2212" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75343,7 +75340,7 @@
         <v>74</v>
       </c>
       <c r="V2212" s="36" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="2213" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75444,7 +75441,7 @@
         <v>74</v>
       </c>
       <c r="V2216" s="36" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="2217" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75476,7 +75473,7 @@
         <v>74</v>
       </c>
       <c r="V2217" s="36" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="2218" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75508,7 +75505,7 @@
         <v>74</v>
       </c>
       <c r="V2218" s="36" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="2219" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75540,7 +75537,7 @@
         <v>74</v>
       </c>
       <c r="V2219" s="36" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="2220" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75596,7 +75593,7 @@
         <v>74</v>
       </c>
       <c r="V2221" s="36" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="2222" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75625,7 +75622,7 @@
         <v>74</v>
       </c>
       <c r="V2222" s="36" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="2223" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75654,7 +75651,7 @@
         <v>74</v>
       </c>
       <c r="V2223" s="36" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="2224" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75683,7 +75680,7 @@
         <v>74</v>
       </c>
       <c r="V2224" s="36" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="2225" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75736,7 +75733,7 @@
         <v>74</v>
       </c>
       <c r="V2226" s="36" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="2227" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75837,7 +75834,7 @@
         <v>74</v>
       </c>
       <c r="V2230" s="36" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="2231" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75914,7 +75911,7 @@
         <v>74</v>
       </c>
       <c r="V2233" s="36" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="2234" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75943,7 +75940,7 @@
         <v>74</v>
       </c>
       <c r="V2234" s="36" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="2235" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75972,7 +75969,7 @@
         <v>74</v>
       </c>
       <c r="V2235" s="36" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="2236" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75995,13 +75992,13 @@
         <v>25</v>
       </c>
       <c r="N2236" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2236" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2236" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2237" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76316,7 +76313,7 @@
         <v>74</v>
       </c>
       <c r="V2249" s="36" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="2250" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76414,7 +76411,7 @@
         <v>1042</v>
       </c>
       <c r="U2253" s="1" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V2253" s="36"/>
     </row>
@@ -76516,7 +76513,7 @@
         <v>74</v>
       </c>
       <c r="V2257" s="36" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="2258" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76545,12 +76542,12 @@
         <v>74</v>
       </c>
       <c r="V2258" s="36" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="2259" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2259" s="6" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="I2259" s="38" t="s">
         <v>65</v>
@@ -76571,13 +76568,13 @@
         <v>23</v>
       </c>
       <c r="N2259" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2259" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2259" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2260" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76676,7 +76673,7 @@
         <v>74</v>
       </c>
       <c r="V2263" s="36" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="2264" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76753,7 +76750,7 @@
         <v>74</v>
       </c>
       <c r="V2266" s="36" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="2267" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76854,7 +76851,7 @@
         <v>74</v>
       </c>
       <c r="V2270" s="36" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="2271" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76883,7 +76880,7 @@
         <v>74</v>
       </c>
       <c r="V2271" s="36" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="2272" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76960,7 +76957,7 @@
         <v>74</v>
       </c>
       <c r="V2274" s="36" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="2275" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77037,7 +77034,7 @@
         <v>74</v>
       </c>
       <c r="V2277" s="36" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="2278" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77066,7 +77063,7 @@
         <v>74</v>
       </c>
       <c r="V2278" s="36" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="2279" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77089,13 +77086,13 @@
         <v>20</v>
       </c>
       <c r="N2279" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2279" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2279" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2280" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77188,13 +77185,13 @@
         <v>4</v>
       </c>
       <c r="N2283" s="36" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="O2283" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2283" s="36" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="2284" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77247,7 +77244,7 @@
         <v>74</v>
       </c>
       <c r="V2285" s="36" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="2286" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77300,7 +77297,7 @@
         <v>74</v>
       </c>
       <c r="V2287" s="36" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="2288" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77353,7 +77350,7 @@
         <v>74</v>
       </c>
       <c r="V2289" s="36" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="2290" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77406,7 +77403,7 @@
         <v>74</v>
       </c>
       <c r="V2291" s="36" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="2292" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77627,7 +77624,7 @@
         <v>74</v>
       </c>
       <c r="V2300" s="36" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="2301" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77650,13 +77647,13 @@
         <v>22</v>
       </c>
       <c r="N2301" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2301" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2301" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2302" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77731,7 +77728,7 @@
         <v>74</v>
       </c>
       <c r="V2304" s="36" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="2305" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77808,7 +77805,7 @@
         <v>74</v>
       </c>
       <c r="V2307" s="36" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="2308" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77885,7 +77882,7 @@
         <v>74</v>
       </c>
       <c r="V2310" s="36" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="2311" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78058,7 +78055,7 @@
         <v>74</v>
       </c>
       <c r="V2317" s="36" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="2318" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78087,7 +78084,7 @@
         <v>74</v>
       </c>
       <c r="V2318" s="36" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="2319" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78110,13 +78107,13 @@
         <v>18</v>
       </c>
       <c r="N2319" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2319" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2319" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2320" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78335,7 +78332,7 @@
         <v>74</v>
       </c>
       <c r="V2328" s="36" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="2329" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78406,7 +78403,7 @@
         <v>12</v>
       </c>
       <c r="N2331" s="37" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="V2331" s="36"/>
     </row>
@@ -78532,7 +78529,7 @@
         <v>74</v>
       </c>
       <c r="V2336" s="36" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="2337" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78579,13 +78576,13 @@
         <v>19</v>
       </c>
       <c r="N2338" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2338" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2338" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78660,7 +78657,7 @@
         <v>74</v>
       </c>
       <c r="V2341" s="36" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="2342" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78761,7 +78758,7 @@
         <v>74</v>
       </c>
       <c r="V2345" s="36" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="2346" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78814,7 +78811,7 @@
         <v>74</v>
       </c>
       <c r="V2347" s="36" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="2348" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78867,7 +78864,7 @@
         <v>74</v>
       </c>
       <c r="V2349" s="36" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="2350" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78944,7 +78941,7 @@
         <v>74</v>
       </c>
       <c r="V2352" s="36" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="2353" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79021,7 +79018,7 @@
         <v>74</v>
       </c>
       <c r="V2355" s="36" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="2356" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79050,7 +79047,7 @@
         <v>74</v>
       </c>
       <c r="V2356" s="36" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="2357" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79079,12 +79076,12 @@
         <v>74</v>
       </c>
       <c r="V2357" s="36" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="2358" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2358" s="6" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="I2358" s="38" t="s">
         <v>70</v>
@@ -79105,13 +79102,13 @@
         <v>20</v>
       </c>
       <c r="N2358" s="36" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="P2358" s="9" t="s">
         <v>75</v>
       </c>
       <c r="V2358" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2359" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79162,7 +79159,7 @@
         <v>74</v>
       </c>
       <c r="V2360" s="36" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="2361" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79191,7 +79188,7 @@
         <v>74</v>
       </c>
       <c r="V2361" s="36" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="2362" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79244,7 +79241,7 @@
         <v>74</v>
       </c>
       <c r="V2363" s="36" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="2364" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79273,7 +79270,7 @@
         <v>74</v>
       </c>
       <c r="V2364" s="36" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="2365" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79326,7 +79323,7 @@
         <v>74</v>
       </c>
       <c r="V2366" s="36" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="2367" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79355,7 +79352,7 @@
         <v>74</v>
       </c>
       <c r="V2367" s="36" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="2368" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79384,7 +79381,7 @@
         <v>74</v>
       </c>
       <c r="V2368" s="36" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="2369" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79413,10 +79410,10 @@
         <v>76</v>
       </c>
       <c r="U2369" s="1" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V2369" s="36" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="2370" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79474,7 +79471,7 @@
         <v>76</v>
       </c>
       <c r="V2371" s="36" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="2372" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79503,7 +79500,7 @@
         <v>76</v>
       </c>
       <c r="V2372" s="36" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2373" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79532,7 +79529,7 @@
         <v>74</v>
       </c>
       <c r="V2373" s="36" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="2374" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79561,7 +79558,7 @@
         <v>76</v>
       </c>
       <c r="V2374" s="36" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="2375" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79619,7 +79616,7 @@
         <v>76</v>
       </c>
       <c r="V2376" s="36" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="2377" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79648,7 +79645,7 @@
         <v>76</v>
       </c>
       <c r="V2377" s="36" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2378" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79677,7 +79674,7 @@
         <v>76</v>
       </c>
       <c r="V2378" s="36" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="2379" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79706,7 +79703,7 @@
         <v>76</v>
       </c>
       <c r="V2379" s="36" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="2380" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79764,7 +79761,7 @@
         <v>76</v>
       </c>
       <c r="V2381" s="36" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="2382" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79793,7 +79790,7 @@
         <v>76</v>
       </c>
       <c r="V2382" s="36" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2383" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79846,7 +79843,7 @@
         <v>74</v>
       </c>
       <c r="V2384" s="36" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="2385" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79899,7 +79896,7 @@
         <v>76</v>
       </c>
       <c r="V2386" s="36" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="2387" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79928,7 +79925,7 @@
         <v>76</v>
       </c>
       <c r="V2387" s="36" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="2388" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79957,7 +79954,7 @@
         <v>76</v>
       </c>
       <c r="V2388" s="36" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="2389" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79983,7 +79980,7 @@
         <v>1117</v>
       </c>
       <c r="U2389" s="1" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="V2389" s="36"/>
     </row>
@@ -80055,7 +80052,7 @@
         <v>34</v>
       </c>
       <c r="N2392" s="36" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="O2392" s="6" t="s">
         <v>74</v>
@@ -80064,7 +80061,7 @@
         <v>75</v>
       </c>
       <c r="V2392" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2393" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80493,7 +80490,7 @@
         <v>74</v>
       </c>
       <c r="V2409" s="36" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="2410" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80570,7 +80567,7 @@
         <v>74</v>
       </c>
       <c r="V2412" s="36" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="2413" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80641,13 +80638,13 @@
         <v>23</v>
       </c>
       <c r="N2415" s="37" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="O2415" s="6" t="s">
         <v>74</v>
       </c>
       <c r="V2415" s="36" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="2416" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80703,7 +80700,7 @@
         <v>75</v>
       </c>
       <c r="V2417" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2418" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81018,7 +81015,7 @@
         <v>74</v>
       </c>
       <c r="V2430" s="36" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="2431" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81095,7 +81092,7 @@
         <v>74</v>
       </c>
       <c r="V2433" s="36" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="2434" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81172,7 +81169,7 @@
         <v>74</v>
       </c>
       <c r="V2436" s="36" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="2437" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81195,7 +81192,7 @@
         <v>20</v>
       </c>
       <c r="N2437" s="36" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="O2437" s="6" t="s">
         <v>74</v>
@@ -81204,7 +81201,7 @@
         <v>75</v>
       </c>
       <c r="V2437" s="36" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="2438" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 25 03 2025
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 5.6 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55F9995-4F77-4B1D-9F31-BDC44676F86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B957E6F-15B3-41F2-B039-733504DE5EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6486" uniqueCount="1522">
   <si>
     <t>Passage</t>
   </si>
@@ -4444,9 +4444,6 @@
   </si>
   <si>
     <t>cakSha#saq itiq cakSha#se</t>
-  </si>
-  <si>
-    <t>naq iti na#H</t>
   </si>
   <si>
     <t>mAqtaraq iti# mAqtara#H</t>
@@ -5242,9 +5239,9 @@
   <dimension ref="A1:V2728"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1889" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1899" sqref="V1899"/>
+      <selection pane="bottomLeft" activeCell="L212" sqref="L212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6838,7 +6835,7 @@
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V27" s="36" t="s">
         <v>1147</v>
@@ -6873,7 +6870,7 @@
         <v>27</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="O28" s="5"/>
       <c r="P28" s="9" t="s">
@@ -7570,7 +7567,7 @@
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
       <c r="U45" s="54" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="V45" s="36"/>
     </row>
@@ -7659,7 +7656,7 @@
       <c r="T47" s="9"/>
       <c r="U47" s="9"/>
       <c r="V47" s="37" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -8623,10 +8620,10 @@
         <v>82</v>
       </c>
       <c r="T71" s="48" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="U71" s="9" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V71" s="36"/>
     </row>
@@ -8672,7 +8669,7 @@
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
       <c r="U72" s="54" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="V72" s="36" t="s">
         <v>1150</v>
@@ -10133,7 +10130,7 @@
       <c r="S109" s="6"/>
       <c r="T109" s="6"/>
       <c r="U109" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V109" s="36"/>
     </row>
@@ -10855,7 +10852,7 @@
       <c r="S127" s="6"/>
       <c r="T127" s="6"/>
       <c r="U127" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V127" s="36"/>
     </row>
@@ -11791,7 +11788,7 @@
       <c r="S152" s="6"/>
       <c r="T152" s="6"/>
       <c r="U152" s="6" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="V152" s="36" t="s">
         <v>1157</v>
@@ -12645,7 +12642,7 @@
       <c r="S174" s="6"/>
       <c r="T174" s="6"/>
       <c r="U174" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V174" s="36"/>
     </row>
@@ -12964,10 +12961,10 @@
       <c r="Q182" s="6"/>
       <c r="R182" s="6"/>
       <c r="S182" s="6" t="s">
+        <v>1498</v>
+      </c>
+      <c r="T182" s="6" t="s">
         <v>1499</v>
-      </c>
-      <c r="T182" s="6" t="s">
-        <v>1500</v>
       </c>
       <c r="U182" s="6"/>
       <c r="V182" s="36"/>
@@ -13575,8 +13572,8 @@
       <c r="S198" s="6"/>
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
-      <c r="V198" s="36" t="s">
-        <v>1472</v>
+      <c r="V198" s="37" t="s">
+        <v>1521</v>
       </c>
     </row>
     <row r="199" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13689,7 +13686,7 @@
       <c r="T201" s="6"/>
       <c r="U201" s="6"/>
       <c r="V201" s="36" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="202" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -13952,7 +13949,7 @@
       <c r="T208" s="6"/>
       <c r="U208" s="6"/>
       <c r="V208" s="36" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="209" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14106,7 +14103,7 @@
       <c r="T212" s="6"/>
       <c r="U212" s="6"/>
       <c r="V212" s="37" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="213" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -14215,7 +14212,7 @@
       <c r="S215" s="6"/>
       <c r="T215" s="6"/>
       <c r="U215" s="6" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="V215" s="36"/>
     </row>
@@ -14520,7 +14517,7 @@
       <c r="T223" s="6"/>
       <c r="U223" s="6"/>
       <c r="V223" s="36" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="224" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24436,7 +24433,7 @@
         <v>291</v>
       </c>
       <c r="N514" s="36" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="O514" s="6" t="s">
         <v>74</v>
@@ -24652,7 +24649,7 @@
       <c r="T520" s="6"/>
       <c r="U520" s="6"/>
       <c r="V520" s="36" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="521" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25660,7 +25657,7 @@
         <v>30</v>
       </c>
       <c r="N550" s="37" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="O550" s="6" t="s">
         <v>74</v>
@@ -28345,7 +28342,7 @@
         <v>108</v>
       </c>
       <c r="N628" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="O628" s="6" t="s">
         <v>74</v>
@@ -28908,7 +28905,7 @@
         <v>124</v>
       </c>
       <c r="N644" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="O644" s="6" t="s">
         <v>74</v>
@@ -29458,7 +29455,7 @@
         <v>140</v>
       </c>
       <c r="N660" s="37" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="O660" s="6" t="s">
         <v>74</v>
@@ -31286,7 +31283,7 @@
     </row>
     <row r="718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A718" s="6" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="I718" s="38" t="s">
         <v>33</v>
@@ -31319,7 +31316,7 @@
       <c r="T718" s="6"/>
       <c r="U718" s="6"/>
       <c r="V718" s="36" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32550,7 +32547,7 @@
     </row>
     <row r="757" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A757" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="I757" s="38" t="s">
         <v>34</v>
@@ -38682,7 +38679,7 @@
     </row>
     <row r="950" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A950" s="6" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="I950" s="38" t="s">
         <v>38</v>
@@ -38715,7 +38712,7 @@
       <c r="T950" s="6"/>
       <c r="U950" s="6"/>
       <c r="V950" s="36" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="951" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38977,7 +38974,7 @@
         <v>83</v>
       </c>
       <c r="T958" s="6" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="U958" s="6"/>
       <c r="V958" s="36"/>
@@ -40510,7 +40507,7 @@
       <c r="T1005" s="6"/>
       <c r="U1005" s="6"/>
       <c r="V1005" s="37" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43683,7 +43680,7 @@
     </row>
     <row r="1104" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1104" s="6" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="H1104" s="25"/>
       <c r="I1104" s="38" t="s">
@@ -43717,7 +43714,7 @@
       <c r="T1104" s="6"/>
       <c r="U1104" s="6"/>
       <c r="V1104" s="36" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1105" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47207,7 +47204,7 @@
         <v>106</v>
       </c>
       <c r="N1210" s="36" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="O1210" s="5"/>
       <c r="P1210" s="6"/>
@@ -47646,7 +47643,7 @@
       <c r="S1223" s="6"/>
       <c r="T1223" s="6"/>
       <c r="U1223" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V1223" s="36" t="s">
         <v>1260</v>
@@ -48818,7 +48815,7 @@
     </row>
     <row r="1261" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1261" s="50" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="I1261" s="38" t="s">
         <v>45</v>
@@ -50511,7 +50508,7 @@
     </row>
     <row r="1314" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1314" s="6" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C1314" s="30"/>
       <c r="I1314" s="38" t="s">
@@ -50545,7 +50542,7 @@
       <c r="T1314" s="6"/>
       <c r="U1314" s="6"/>
       <c r="V1314" s="36" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1315" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52684,7 +52681,7 @@
       <c r="T1377" s="6"/>
       <c r="U1377" s="6"/>
       <c r="V1377" s="37" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="1378" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52753,7 +52750,7 @@
       <c r="T1379" s="6"/>
       <c r="U1379" s="6"/>
       <c r="V1379" s="37" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53596,7 +53593,7 @@
         <v>90</v>
       </c>
       <c r="N1404" s="37" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="O1404" s="6" t="s">
         <v>74</v>
@@ -56541,7 +56538,7 @@
       <c r="T1492" s="6"/>
       <c r="U1492" s="6"/>
       <c r="V1492" s="36" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1493" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62442,7 +62439,7 @@
         <v>110</v>
       </c>
       <c r="T1700" s="1" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="V1700" s="36"/>
     </row>
@@ -64399,7 +64396,7 @@
     </row>
     <row r="1780" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1780" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="I1780" s="38" t="s">
         <v>54</v>
@@ -64901,7 +64898,7 @@
         <v>75</v>
       </c>
       <c r="V1799" s="36" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1800" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65993,7 +65990,7 @@
         <v>83</v>
       </c>
       <c r="T1843" s="6" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="V1843" s="36"/>
     </row>
@@ -69148,7 +69145,7 @@
         <v>75</v>
       </c>
       <c r="V1969" s="36" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1970" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71194,7 +71191,7 @@
         <v>83</v>
       </c>
       <c r="N2052" s="37" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="O2052" s="6" t="s">
         <v>74</v>
@@ -73260,7 +73257,7 @@
     </row>
     <row r="2134" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2134" s="6" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="I2134" s="38" t="s">
         <v>60</v>
@@ -73287,7 +73284,7 @@
         <v>75</v>
       </c>
       <c r="V2134" s="36" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="2135" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73964,7 +73961,7 @@
         <v>75</v>
       </c>
       <c r="V2160" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2161" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74293,7 +74290,7 @@
         <v>13</v>
       </c>
       <c r="N2173" s="37" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="O2173" s="6" t="s">
         <v>74</v>
@@ -74631,7 +74628,7 @@
         <v>75</v>
       </c>
       <c r="V2186" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2187" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75313,7 +75310,7 @@
         <v>75</v>
       </c>
       <c r="V2211" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2212" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -75998,7 +75995,7 @@
         <v>75</v>
       </c>
       <c r="V2236" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2237" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -76411,7 +76408,7 @@
         <v>1042</v>
       </c>
       <c r="U2253" s="1" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="V2253" s="36"/>
     </row>
@@ -76547,7 +76544,7 @@
     </row>
     <row r="2259" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2259" s="6" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="I2259" s="38" t="s">
         <v>65</v>
@@ -76574,7 +76571,7 @@
         <v>75</v>
       </c>
       <c r="V2259" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2260" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77092,7 +77089,7 @@
         <v>75</v>
       </c>
       <c r="V2279" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2280" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -77185,7 +77182,7 @@
         <v>4</v>
       </c>
       <c r="N2283" s="36" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="O2283" s="6" t="s">
         <v>74</v>
@@ -77653,7 +77650,7 @@
         <v>75</v>
       </c>
       <c r="V2301" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2302" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78113,7 +78110,7 @@
         <v>75</v>
       </c>
       <c r="V2319" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2320" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78403,7 +78400,7 @@
         <v>12</v>
       </c>
       <c r="N2331" s="37" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="V2331" s="36"/>
     </row>
@@ -78582,7 +78579,7 @@
         <v>75</v>
       </c>
       <c r="V2338" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79081,7 +79078,7 @@
     </row>
     <row r="2358" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2358" s="6" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="I2358" s="38" t="s">
         <v>70</v>
@@ -79108,7 +79105,7 @@
         <v>75</v>
       </c>
       <c r="V2358" s="36" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="2359" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -79410,7 +79407,7 @@
         <v>76</v>
       </c>
       <c r="U2369" s="1" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="V2369" s="36" t="s">
         <v>1412</v>
@@ -79980,7 +79977,7 @@
         <v>1117</v>
       </c>
       <c r="U2389" s="1" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="V2389" s="36"/>
     </row>
@@ -80061,7 +80058,7 @@
         <v>75</v>
       </c>
       <c r="V2392" s="36" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="2393" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -80638,7 +80635,7 @@
         <v>23</v>
       </c>
       <c r="N2415" s="37" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="O2415" s="6" t="s">
         <v>74</v>
@@ -80700,7 +80697,7 @@
         <v>75</v>
       </c>
       <c r="V2417" s="36" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="2418" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -81201,7 +81198,7 @@
         <v>75</v>
       </c>
       <c r="V2437" s="36" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="2438" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>